<commit_message>
get half of it done
</commit_message>
<xml_diff>
--- a/doc/设备通讯协议.xlsx
+++ b/doc/设备通讯协议.xlsx
@@ -513,18 +513,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>准备好接OK板</t>
-  </si>
-  <si>
     <t>等待暂存机返回“准备好接OK板”指令：52 c2 04 19</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>等待暂存机返回“准备好接NG板”指令：52 c2 05 1a</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>准备好接NG板</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -603,6 +596,14 @@
     <t xml:space="preserve">    第一字节数据头；第二字节为命令，当小于0xc0表示数据；第三字节为参数;第四字节为前面三字节之和，取低字节。
     第二字节与第三字节组合表示调节导轨的宽度值，取值范围为0x0000-0x3fff，数值0x0001调节的宽度值为0.025mm。
 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>准备好接NG板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>准备好接OK板</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -920,26 +921,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -948,6 +931,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1417,8 +1418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1435,47 +1436,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5" x14ac:dyDescent="0.15">
-      <c r="A1" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="A1" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="A2" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34" t="s">
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
     </row>
     <row r="4" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A4" s="33"/>
+      <c r="A4" s="35"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1485,7 +1486,7 @@
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="34"/>
+      <c r="E4" s="36"/>
       <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1501,7 +1502,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>76</v>
@@ -1509,7 +1510,7 @@
       <c r="D5" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="34"/>
+      <c r="E5" s="36"/>
       <c r="F5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1531,7 +1532,7 @@
       <c r="D6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="34"/>
+      <c r="E6" s="36"/>
       <c r="F6" s="2" t="s">
         <v>20</v>
       </c>
@@ -1553,7 +1554,7 @@
       <c r="D7" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E7" s="34"/>
+      <c r="E7" s="36"/>
       <c r="F7" s="2" t="s">
         <v>90</v>
       </c>
@@ -1568,10 +1569,10 @@
         <v>108</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D8" s="5"/>
-      <c r="E8" s="34"/>
+      <c r="E8" s="36"/>
       <c r="F8" s="2" t="s">
         <v>59</v>
       </c>
@@ -1591,7 +1592,7 @@
         <v>80</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="34"/>
+      <c r="E9" s="36"/>
       <c r="F9" s="2" t="s">
         <v>97</v>
       </c>
@@ -1608,10 +1609,10 @@
         <v>63</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D10" s="6"/>
-      <c r="E10" s="34"/>
+      <c r="E10" s="36"/>
       <c r="F10" s="2" t="s">
         <v>27</v>
       </c>
@@ -1631,12 +1632,12 @@
         <v>35</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="34"/>
+      <c r="E11" s="36"/>
       <c r="F11" s="27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
@@ -1650,12 +1651,12 @@
         <v>111</v>
       </c>
       <c r="D12" s="22"/>
-      <c r="E12" s="34"/>
+      <c r="E12" s="36"/>
       <c r="F12" s="22" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H12" s="2"/>
     </row>
@@ -1670,12 +1671,12 @@
         <v>116</v>
       </c>
       <c r="D13" s="22"/>
-      <c r="E13" s="34"/>
+      <c r="E13" s="36"/>
       <c r="F13" s="22" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H13" s="2"/>
     </row>
@@ -1687,15 +1688,15 @@
         <v>64</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="34"/>
+      <c r="E14" s="36"/>
       <c r="F14" s="22" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H14" s="2"/>
     </row>
@@ -1707,15 +1708,15 @@
         <v>8</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D15" s="2"/>
-      <c r="E15" s="34"/>
+      <c r="E15" s="36"/>
       <c r="F15" s="22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G15" s="22" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H15" s="2"/>
     </row>
@@ -1727,10 +1728,10 @@
         <v>9</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="34"/>
+      <c r="E16" s="36"/>
       <c r="F16" s="2" t="s">
         <v>92</v>
       </c>
@@ -1752,7 +1753,7 @@
       <c r="D17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E17" s="34"/>
+      <c r="E17" s="36"/>
       <c r="F17" s="2" t="s">
         <v>53</v>
       </c>
@@ -1768,7 +1769,7 @@
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="34"/>
+      <c r="E18" s="36"/>
       <c r="F18" s="2" t="s">
         <v>54</v>
       </c>
@@ -1784,7 +1785,7 @@
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="34"/>
+      <c r="E19" s="36"/>
       <c r="F19" s="2" t="s">
         <v>31</v>
       </c>
@@ -1800,7 +1801,7 @@
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
-      <c r="E20" s="34"/>
+      <c r="E20" s="36"/>
       <c r="F20" s="2" t="s">
         <v>32</v>
       </c>
@@ -1816,7 +1817,7 @@
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
-      <c r="E21" s="34"/>
+      <c r="E21" s="36"/>
       <c r="F21" s="2" t="s">
         <v>33</v>
       </c>
@@ -1832,7 +1833,7 @@
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="34"/>
+      <c r="E22" s="36"/>
       <c r="F22" s="2" t="s">
         <v>34</v>
       </c>
@@ -1848,7 +1849,7 @@
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
-      <c r="E23" s="34"/>
+      <c r="E23" s="36"/>
       <c r="F23" s="2" t="s">
         <v>57</v>
       </c>
@@ -1866,12 +1867,12 @@
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
-      <c r="E24" s="34"/>
+      <c r="E24" s="36"/>
       <c r="F24" s="2" t="s">
         <v>57</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H24" s="2"/>
     </row>
@@ -1882,7 +1883,7 @@
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="34"/>
+      <c r="E25" s="36"/>
       <c r="F25" s="2" t="s">
         <v>57</v>
       </c>
@@ -1900,7 +1901,7 @@
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="34"/>
+      <c r="E26" s="36"/>
       <c r="F26" s="2" t="s">
         <v>57</v>
       </c>
@@ -1918,12 +1919,12 @@
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="34"/>
+      <c r="E27" s="36"/>
       <c r="F27" s="22" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G27" s="22" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H27" s="2"/>
     </row>
@@ -1934,22 +1935,22 @@
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="34"/>
+      <c r="E28" s="36"/>
       <c r="F28" s="19"/>
       <c r="G28" s="19"/>
       <c r="H28" s="19"/>
     </row>
     <row r="29" spans="1:9" s="16" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
     </row>
     <row r="30" spans="1:9" s="16" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A30" s="4"/>
@@ -1965,18 +1966,18 @@
       <c r="A31" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
     </row>
     <row r="32" spans="1:9" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="29" t="s">
         <v>10</v>
       </c>
       <c r="C32" s="18" t="s">
@@ -2002,7 +2003,7 @@
       </c>
     </row>
     <row r="33" spans="2:9" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="B33" s="36"/>
+      <c r="B33" s="30"/>
       <c r="C33" s="18" t="s">
         <v>85</v>
       </c>
@@ -2190,8 +2191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:F39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2228,7 +2229,7 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
@@ -2282,7 +2283,7 @@
         <v>3</v>
       </c>
       <c r="F23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
add flow in doc
</commit_message>
<xml_diff>
--- a/doc/设备通讯协议.xlsx
+++ b/doc/设备通讯协议.xlsx
@@ -11,7 +11,7 @@
     <sheet name="暂存机" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -355,7 +355,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="208">
   <si>
     <t>序号</t>
   </si>
@@ -1199,6 +1199,22 @@
   </si>
   <si>
     <t>测试OK准备送板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发送送板指令给上一个设备</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>检测上一个设备是否处于等待状态</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1506,7 +1522,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1608,6 +1624,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1644,30 +1666,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1676,7 +1698,10 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -9781,6 +9806,1513 @@
         <a:xfrm>
           <a:off x="16843172" y="7304309"/>
           <a:ext cx="417785" cy="952"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>336173</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>161696</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>7998</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="226" name="直接箭头连接符 225"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="228" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="16741585" y="12768314"/>
+          <a:ext cx="355384" cy="6392"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>7998</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>7998</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>155304</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="228" name="流程图: 决策 227"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17096969" y="12438529"/>
+          <a:ext cx="2050676" cy="659569"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1600"/>
+            <a:t>是否等待</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>355382</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>11208</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>340092</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>162714</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="230" name="椭圆 229"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17444353" y="13794443"/>
+          <a:ext cx="1351827" cy="1328124"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1600"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1500" b="1"/>
+            <a:t>送板指令</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1500" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>344178</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>349940</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>16350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="231" name="直接箭头连接符 230"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="18116707" y="13110882"/>
+          <a:ext cx="5762" cy="688703"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>155304</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="235" name="流程图: 决策 234"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8202706" y="12438529"/>
+          <a:ext cx="2050676" cy="659569"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1600"/>
+            <a:t>是否等待</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>347384</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>11208</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>332093</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>162714</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="246" name="椭圆 245"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8550090" y="13794443"/>
+          <a:ext cx="1351827" cy="1328124"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1600"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1500" b="1"/>
+            <a:t>送板指令</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1500" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>336179</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>341941</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>16350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="248" name="直接箭头连接符 247"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="9222444" y="13110882"/>
+          <a:ext cx="5762" cy="688703"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>161696</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>347671</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>694</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="63" name="直接箭头连接符 62"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="40" idx="1"/>
+          <a:endCxn id="235" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="10253382" y="12768314"/>
+          <a:ext cx="347671" cy="7086"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>326570</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>161697</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>678753</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="198" name="直接箭头连接符 197"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="201" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="27540856" y="12013518"/>
+          <a:ext cx="352183" cy="15197"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>678753</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>678753</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>155305</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="201" name="流程图: 决策 200"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="27893039" y="11674929"/>
+          <a:ext cx="2041071" cy="685983"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1600"/>
+            <a:t>是否等待</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>345780</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>11209</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>330490</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>162715</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="202" name="椭圆 201"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="28240423" y="13101280"/>
+          <a:ext cx="1345424" cy="1389756"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1600"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1500" b="1"/>
+            <a:t>送板指令</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1500" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>334576</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>340338</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>16351</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="203" name="直接箭头连接符 202"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="28909576" y="12382501"/>
+          <a:ext cx="5762" cy="723921"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>155305</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="208" name="流程图: 决策 207"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19050000" y="17689286"/>
+          <a:ext cx="2041071" cy="685983"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1600"/>
+            <a:t>是否等待</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>347384</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>11208</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>332093</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>162714</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="209" name="椭圆 208"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19397384" y="19115637"/>
+          <a:ext cx="1345423" cy="1389756"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1600"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1500" b="1"/>
+            <a:t>送板指令</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1500" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>336179</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>341941</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>16350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="219" name="直接箭头连接符 218"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="20066536" y="18396858"/>
+          <a:ext cx="5762" cy="723921"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>161696</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>347671</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>695</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="232" name="直接箭头连接符 231"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="208" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="21091071" y="18027875"/>
+          <a:ext cx="347671" cy="15891"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>52</xdr:col>
+      <xdr:colOff>347671</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>164244</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>352183</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>171330</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="233" name="直接箭头连接符 232"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="113" idx="3"/>
+          <a:endCxn id="234" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="36369489" y="13152880"/>
+          <a:ext cx="697239" cy="7086"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>352183</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>352183</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>155305</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="234" name="流程图: 决策 233"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="37066728" y="12815455"/>
+          <a:ext cx="2078182" cy="674850"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1600"/>
+            <a:t>是否等待</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>19209</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>11210</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>3920</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>162715</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="249" name="椭圆 248"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="37426482" y="14212119"/>
+          <a:ext cx="1370165" cy="1363778"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1600"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1500" b="1"/>
+            <a:t>送板指令</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1500" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>8005</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>13767</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>16352</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="250" name="直接箭头连接符 249"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="38108005" y="13508183"/>
+          <a:ext cx="5762" cy="709078"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>76</xdr:col>
+      <xdr:colOff>294412</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>164243</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>77</xdr:col>
+      <xdr:colOff>298924</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>171329</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="251" name="直接箭头连接符 250"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="252" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="52941685" y="21119243"/>
+          <a:ext cx="697239" cy="7086"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>77</xdr:col>
+      <xdr:colOff>298924</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>80</xdr:col>
+      <xdr:colOff>298924</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>155304</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="252" name="流程图: 决策 251"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="53638924" y="20781818"/>
+          <a:ext cx="2078182" cy="674850"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1600"/>
+            <a:t>是否等待</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>77</xdr:col>
+      <xdr:colOff>658678</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>11209</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>79</xdr:col>
+      <xdr:colOff>643388</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>162715</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="253" name="椭圆 252"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="53998678" y="22178482"/>
+          <a:ext cx="1370165" cy="1363778"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1600"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1500" b="1"/>
+            <a:t>送板指令</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1500" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>78</xdr:col>
+      <xdr:colOff>647474</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>78</xdr:col>
+      <xdr:colOff>653236</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>16351</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="254" name="直接箭头连接符 253"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="54680201" y="21474546"/>
+          <a:ext cx="5762" cy="709078"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>66</xdr:col>
+      <xdr:colOff>692726</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>155304</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="262" name="流程图: 决策 261"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="44334545" y="20781818"/>
+          <a:ext cx="2078181" cy="674850"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1600"/>
+            <a:t>是否等待</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>347384</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>11207</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>66</xdr:col>
+      <xdr:colOff>332092</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>162714</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="283" name="椭圆 282"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="44681929" y="22178480"/>
+          <a:ext cx="1370163" cy="1363779"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1600"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1500" b="1"/>
+            <a:t>送板指令</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1500" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>65</xdr:col>
+      <xdr:colOff>336178</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>65</xdr:col>
+      <xdr:colOff>341940</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>16349</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="284" name="直接箭头连接符 283"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="45363451" y="21474546"/>
+          <a:ext cx="5762" cy="709076"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>66</xdr:col>
+      <xdr:colOff>692726</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>161696</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>67</xdr:col>
+      <xdr:colOff>347670</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>694</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="285" name="直接箭头连接符 284"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="262" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="46412726" y="21116696"/>
+          <a:ext cx="347671" cy="12180"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -10098,8 +11630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -10116,47 +11648,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5" x14ac:dyDescent="0.15">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
     </row>
     <row r="3" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40" t="s">
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
     </row>
     <row r="4" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A4" s="39"/>
+      <c r="A4" s="41"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -10166,7 +11698,7 @@
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="40"/>
+      <c r="E4" s="42"/>
       <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
@@ -10190,7 +11722,7 @@
       <c r="D5" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="40"/>
+      <c r="E5" s="42"/>
       <c r="F5" s="2" t="s">
         <v>6</v>
       </c>
@@ -10212,7 +11744,7 @@
       <c r="D6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="40"/>
+      <c r="E6" s="42"/>
       <c r="F6" s="2" t="s">
         <v>20</v>
       </c>
@@ -10234,7 +11766,7 @@
       <c r="D7" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E7" s="40"/>
+      <c r="E7" s="42"/>
       <c r="F7" s="2" t="s">
         <v>90</v>
       </c>
@@ -10252,7 +11784,7 @@
         <v>124</v>
       </c>
       <c r="D8" s="5"/>
-      <c r="E8" s="40"/>
+      <c r="E8" s="42"/>
       <c r="F8" s="2" t="s">
         <v>59</v>
       </c>
@@ -10272,7 +11804,7 @@
         <v>80</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="40"/>
+      <c r="E9" s="42"/>
       <c r="F9" s="2" t="s">
         <v>97</v>
       </c>
@@ -10292,7 +11824,7 @@
         <v>133</v>
       </c>
       <c r="D10" s="6"/>
-      <c r="E10" s="40"/>
+      <c r="E10" s="42"/>
       <c r="F10" s="2" t="s">
         <v>27</v>
       </c>
@@ -10312,7 +11844,7 @@
         <v>35</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="40"/>
+      <c r="E11" s="42"/>
       <c r="F11" s="27" t="s">
         <v>145</v>
       </c>
@@ -10331,7 +11863,7 @@
         <v>111</v>
       </c>
       <c r="D12" s="22"/>
-      <c r="E12" s="40"/>
+      <c r="E12" s="42"/>
       <c r="F12" s="22" t="s">
         <v>138</v>
       </c>
@@ -10351,7 +11883,7 @@
         <v>116</v>
       </c>
       <c r="D13" s="22"/>
-      <c r="E13" s="40"/>
+      <c r="E13" s="42"/>
       <c r="F13" s="22" t="s">
         <v>137</v>
       </c>
@@ -10371,7 +11903,7 @@
         <v>131</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="40"/>
+      <c r="E14" s="42"/>
       <c r="F14" s="22" t="s">
         <v>123</v>
       </c>
@@ -10391,7 +11923,7 @@
         <v>130</v>
       </c>
       <c r="D15" s="2"/>
-      <c r="E15" s="40"/>
+      <c r="E15" s="42"/>
       <c r="F15" s="22" t="s">
         <v>122</v>
       </c>
@@ -10411,7 +11943,7 @@
         <v>132</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="40"/>
+      <c r="E16" s="42"/>
       <c r="F16" s="2" t="s">
         <v>92</v>
       </c>
@@ -10433,7 +11965,7 @@
       <c r="D17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E17" s="40"/>
+      <c r="E17" s="42"/>
       <c r="F17" s="2" t="s">
         <v>53</v>
       </c>
@@ -10449,7 +11981,7 @@
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="40"/>
+      <c r="E18" s="42"/>
       <c r="F18" s="2" t="s">
         <v>54</v>
       </c>
@@ -10465,7 +11997,7 @@
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="40"/>
+      <c r="E19" s="42"/>
       <c r="F19" s="2" t="s">
         <v>143</v>
       </c>
@@ -10481,7 +12013,7 @@
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
-      <c r="E20" s="40"/>
+      <c r="E20" s="42"/>
       <c r="F20" s="2" t="s">
         <v>32</v>
       </c>
@@ -10497,7 +12029,7 @@
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
-      <c r="E21" s="40"/>
+      <c r="E21" s="42"/>
       <c r="F21" s="2" t="s">
         <v>33</v>
       </c>
@@ -10513,7 +12045,7 @@
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="40"/>
+      <c r="E22" s="42"/>
       <c r="F22" s="2" t="s">
         <v>34</v>
       </c>
@@ -10529,7 +12061,7 @@
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
-      <c r="E23" s="40"/>
+      <c r="E23" s="42"/>
       <c r="F23" s="2" t="s">
         <v>57</v>
       </c>
@@ -10547,7 +12079,7 @@
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
-      <c r="E24" s="40"/>
+      <c r="E24" s="42"/>
       <c r="F24" s="2" t="s">
         <v>57</v>
       </c>
@@ -10563,7 +12095,7 @@
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="40"/>
+      <c r="E25" s="42"/>
       <c r="F25" s="2" t="s">
         <v>57</v>
       </c>
@@ -10581,7 +12113,7 @@
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="40"/>
+      <c r="E26" s="42"/>
       <c r="F26" s="2" t="s">
         <v>57</v>
       </c>
@@ -10599,7 +12131,7 @@
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="40"/>
+      <c r="E27" s="42"/>
       <c r="F27" s="22" t="s">
         <v>120</v>
       </c>
@@ -10615,22 +12147,22 @@
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="40"/>
+      <c r="E28" s="42"/>
       <c r="F28" s="19"/>
       <c r="G28" s="19"/>
       <c r="H28" s="19"/>
     </row>
     <row r="29" spans="1:9" s="16" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="35"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
     </row>
     <row r="30" spans="1:9" s="16" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A30" s="4"/>
@@ -10646,18 +12178,18 @@
       <c r="A31" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="32" t="s">
+      <c r="B31" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
     </row>
     <row r="32" spans="1:9" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="B32" s="33" t="s">
+      <c r="B32" s="35" t="s">
         <v>10</v>
       </c>
       <c r="C32" s="18" t="s">
@@ -10683,7 +12215,7 @@
       </c>
     </row>
     <row r="33" spans="2:9" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="B33" s="34"/>
+      <c r="B33" s="36"/>
       <c r="C33" s="18" t="s">
         <v>85</v>
       </c>
@@ -10987,24 +12519,24 @@
       </c>
     </row>
     <row r="39" spans="1:6" s="24" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="41" t="s">
+      <c r="A39" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="B39" s="41"/>
-      <c r="C39" s="41"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="41"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="43"/>
+      <c r="D39" s="43"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="43"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>109</v>
       </c>
-      <c r="C40" s="42" t="s">
+      <c r="C40" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="D40" s="42"/>
-      <c r="E40" s="42"/>
+      <c r="D40" s="44"/>
+      <c r="E40" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -11020,10 +12552,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:CU108"/>
+  <dimension ref="A5:CU212"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
-      <selection activeCell="AZ80" sqref="AZ80:BE81"/>
+      <selection activeCell="AV80" sqref="AV80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -11079,172 +12611,172 @@
       </c>
     </row>
     <row r="16" spans="3:90" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C16" s="43" t="s">
+      <c r="C16" s="48" t="s">
         <v>152</v>
       </c>
-      <c r="D16" s="42"/>
-      <c r="T16" s="43" t="s">
+      <c r="D16" s="44"/>
+      <c r="T16" s="48" t="s">
         <v>162</v>
       </c>
-      <c r="U16" s="43"/>
-      <c r="AJ16" s="43" t="s">
+      <c r="U16" s="48"/>
+      <c r="AJ16" s="48" t="s">
         <v>176</v>
       </c>
-      <c r="AK16" s="43"/>
-      <c r="AY16" s="43" t="s">
+      <c r="AK16" s="48"/>
+      <c r="AY16" s="48" t="s">
         <v>171</v>
       </c>
-      <c r="AZ16" s="43"/>
-      <c r="BT16" s="43" t="s">
+      <c r="AZ16" s="48"/>
+      <c r="BT16" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="BU16" s="43"/>
-      <c r="CK16" s="43" t="s">
+      <c r="BU16" s="48"/>
+      <c r="CK16" s="48" t="s">
         <v>198</v>
       </c>
-      <c r="CL16" s="43"/>
+      <c r="CL16" s="48"/>
     </row>
     <row r="17" spans="3:97" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="T17" s="43"/>
-      <c r="U17" s="43"/>
-      <c r="AJ17" s="43"/>
-      <c r="AK17" s="43"/>
-      <c r="AY17" s="43"/>
-      <c r="AZ17" s="43"/>
-      <c r="BT17" s="43"/>
-      <c r="BU17" s="43"/>
-      <c r="CK17" s="43"/>
-      <c r="CL17" s="43"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="T17" s="48"/>
+      <c r="U17" s="48"/>
+      <c r="AJ17" s="48"/>
+      <c r="AK17" s="48"/>
+      <c r="AY17" s="48"/>
+      <c r="AZ17" s="48"/>
+      <c r="BT17" s="48"/>
+      <c r="BU17" s="48"/>
+      <c r="CK17" s="48"/>
+      <c r="CL17" s="48"/>
     </row>
     <row r="19" spans="3:97" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E19" s="43" t="s">
+      <c r="E19" s="48" t="s">
         <v>153</v>
       </c>
-      <c r="F19" s="42"/>
-      <c r="V19" s="43" t="s">
+      <c r="F19" s="44"/>
+      <c r="V19" s="48" t="s">
         <v>163</v>
       </c>
-      <c r="W19" s="42"/>
-      <c r="X19" s="42"/>
-      <c r="Y19" s="42"/>
-      <c r="Z19" s="42"/>
-      <c r="AA19" s="42"/>
-      <c r="AB19" s="42"/>
-      <c r="AL19" s="43" t="s">
+      <c r="W19" s="44"/>
+      <c r="X19" s="44"/>
+      <c r="Y19" s="44"/>
+      <c r="Z19" s="44"/>
+      <c r="AA19" s="44"/>
+      <c r="AB19" s="44"/>
+      <c r="AL19" s="48" t="s">
         <v>177</v>
       </c>
-      <c r="AM19" s="42"/>
-      <c r="AN19" s="42"/>
-      <c r="AO19" s="42"/>
-      <c r="AP19" s="42"/>
-      <c r="AQ19" s="42"/>
-      <c r="AR19" s="42"/>
+      <c r="AM19" s="44"/>
+      <c r="AN19" s="44"/>
+      <c r="AO19" s="44"/>
+      <c r="AP19" s="44"/>
+      <c r="AQ19" s="44"/>
+      <c r="AR19" s="44"/>
       <c r="AS19" s="46"/>
       <c r="AT19" s="46"/>
       <c r="AU19" s="46"/>
-      <c r="BA19" s="43" t="s">
+      <c r="BA19" s="48" t="s">
         <v>163</v>
       </c>
-      <c r="BB19" s="42"/>
-      <c r="BC19" s="42"/>
-      <c r="BD19" s="42"/>
-      <c r="BE19" s="42"/>
-      <c r="BF19" s="42"/>
-      <c r="BG19" s="42"/>
-      <c r="BV19" s="43" t="s">
+      <c r="BB19" s="44"/>
+      <c r="BC19" s="44"/>
+      <c r="BD19" s="44"/>
+      <c r="BE19" s="44"/>
+      <c r="BF19" s="44"/>
+      <c r="BG19" s="44"/>
+      <c r="BV19" s="48" t="s">
         <v>163</v>
       </c>
-      <c r="BW19" s="42"/>
-      <c r="BX19" s="42"/>
-      <c r="BY19" s="42"/>
-      <c r="BZ19" s="42"/>
-      <c r="CA19" s="42"/>
-      <c r="CB19" s="42"/>
-      <c r="CM19" s="43" t="s">
+      <c r="BW19" s="44"/>
+      <c r="BX19" s="44"/>
+      <c r="BY19" s="44"/>
+      <c r="BZ19" s="44"/>
+      <c r="CA19" s="44"/>
+      <c r="CB19" s="44"/>
+      <c r="CM19" s="48" t="s">
         <v>163</v>
       </c>
-      <c r="CN19" s="42"/>
-      <c r="CO19" s="42"/>
-      <c r="CP19" s="42"/>
-      <c r="CQ19" s="42"/>
-      <c r="CR19" s="42"/>
-      <c r="CS19" s="42"/>
+      <c r="CN19" s="44"/>
+      <c r="CO19" s="44"/>
+      <c r="CP19" s="44"/>
+      <c r="CQ19" s="44"/>
+      <c r="CR19" s="44"/>
+      <c r="CS19" s="44"/>
     </row>
     <row r="20" spans="3:97" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="V20" s="42"/>
-      <c r="W20" s="42"/>
-      <c r="X20" s="42"/>
-      <c r="Y20" s="42"/>
-      <c r="Z20" s="42"/>
-      <c r="AA20" s="42"/>
-      <c r="AB20" s="42"/>
-      <c r="AL20" s="42"/>
-      <c r="AM20" s="42"/>
-      <c r="AN20" s="42"/>
-      <c r="AO20" s="42"/>
-      <c r="AP20" s="42"/>
-      <c r="AQ20" s="42"/>
-      <c r="AR20" s="42"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="V20" s="44"/>
+      <c r="W20" s="44"/>
+      <c r="X20" s="44"/>
+      <c r="Y20" s="44"/>
+      <c r="Z20" s="44"/>
+      <c r="AA20" s="44"/>
+      <c r="AB20" s="44"/>
+      <c r="AL20" s="44"/>
+      <c r="AM20" s="44"/>
+      <c r="AN20" s="44"/>
+      <c r="AO20" s="44"/>
+      <c r="AP20" s="44"/>
+      <c r="AQ20" s="44"/>
+      <c r="AR20" s="44"/>
       <c r="AS20" s="46"/>
       <c r="AT20" s="46"/>
       <c r="AU20" s="46"/>
-      <c r="BA20" s="42"/>
-      <c r="BB20" s="42"/>
-      <c r="BC20" s="42"/>
-      <c r="BD20" s="42"/>
-      <c r="BE20" s="42"/>
-      <c r="BF20" s="42"/>
-      <c r="BG20" s="42"/>
-      <c r="BV20" s="42"/>
-      <c r="BW20" s="42"/>
-      <c r="BX20" s="42"/>
-      <c r="BY20" s="42"/>
-      <c r="BZ20" s="42"/>
-      <c r="CA20" s="42"/>
-      <c r="CB20" s="42"/>
-      <c r="CM20" s="42"/>
-      <c r="CN20" s="42"/>
-      <c r="CO20" s="42"/>
-      <c r="CP20" s="42"/>
-      <c r="CQ20" s="42"/>
-      <c r="CR20" s="42"/>
-      <c r="CS20" s="42"/>
+      <c r="BA20" s="44"/>
+      <c r="BB20" s="44"/>
+      <c r="BC20" s="44"/>
+      <c r="BD20" s="44"/>
+      <c r="BE20" s="44"/>
+      <c r="BF20" s="44"/>
+      <c r="BG20" s="44"/>
+      <c r="BV20" s="44"/>
+      <c r="BW20" s="44"/>
+      <c r="BX20" s="44"/>
+      <c r="BY20" s="44"/>
+      <c r="BZ20" s="44"/>
+      <c r="CA20" s="44"/>
+      <c r="CB20" s="44"/>
+      <c r="CM20" s="44"/>
+      <c r="CN20" s="44"/>
+      <c r="CO20" s="44"/>
+      <c r="CP20" s="44"/>
+      <c r="CQ20" s="44"/>
+      <c r="CR20" s="44"/>
+      <c r="CS20" s="44"/>
     </row>
     <row r="23" spans="3:97" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D23" s="44" t="s">
+      <c r="D23" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="E23" s="45"/>
+      <c r="E23" s="50"/>
       <c r="F23" s="46"/>
       <c r="G23" s="46"/>
       <c r="H23" s="46"/>
       <c r="I23" s="46"/>
-      <c r="U23" s="44" t="s">
+      <c r="U23" s="45" t="s">
         <v>164</v>
       </c>
-      <c r="V23" s="44"/>
-      <c r="W23" s="44"/>
-      <c r="X23" s="44"/>
-      <c r="Y23" s="44"/>
-      <c r="Z23" s="44"/>
+      <c r="V23" s="45"/>
+      <c r="W23" s="45"/>
+      <c r="X23" s="45"/>
+      <c r="Y23" s="45"/>
+      <c r="Z23" s="45"/>
       <c r="AK23" s="30"/>
       <c r="AL23" s="30"/>
       <c r="AM23" s="30"/>
       <c r="AN23" s="30"/>
       <c r="AO23" s="30"/>
       <c r="AP23" s="30"/>
-      <c r="AZ23" s="44" t="s">
+      <c r="AZ23" s="45" t="s">
         <v>164</v>
       </c>
-      <c r="BA23" s="44"/>
-      <c r="BB23" s="44"/>
-      <c r="BC23" s="44"/>
-      <c r="BD23" s="44"/>
-      <c r="BE23" s="44"/>
+      <c r="BA23" s="45"/>
+      <c r="BB23" s="45"/>
+      <c r="BC23" s="45"/>
+      <c r="BD23" s="45"/>
+      <c r="BE23" s="45"/>
       <c r="BU23" s="30"/>
       <c r="BV23" s="30"/>
       <c r="BW23" s="30"/>
@@ -11259,30 +12791,30 @@
       <c r="CQ23" s="30"/>
     </row>
     <row r="24" spans="3:97" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
       <c r="F24" s="46"/>
       <c r="G24" s="46"/>
       <c r="H24" s="46"/>
       <c r="I24" s="46"/>
-      <c r="U24" s="44"/>
-      <c r="V24" s="44"/>
-      <c r="W24" s="44"/>
-      <c r="X24" s="44"/>
-      <c r="Y24" s="44"/>
-      <c r="Z24" s="44"/>
+      <c r="U24" s="45"/>
+      <c r="V24" s="45"/>
+      <c r="W24" s="45"/>
+      <c r="X24" s="45"/>
+      <c r="Y24" s="45"/>
+      <c r="Z24" s="45"/>
       <c r="AK24" s="30"/>
       <c r="AL24" s="30"/>
       <c r="AM24" s="30"/>
       <c r="AN24" s="30"/>
       <c r="AO24" s="30"/>
       <c r="AP24" s="30"/>
-      <c r="AZ24" s="44"/>
-      <c r="BA24" s="44"/>
-      <c r="BB24" s="44"/>
-      <c r="BC24" s="44"/>
-      <c r="BD24" s="44"/>
-      <c r="BE24" s="44"/>
+      <c r="AZ24" s="45"/>
+      <c r="BA24" s="45"/>
+      <c r="BB24" s="45"/>
+      <c r="BC24" s="45"/>
+      <c r="BD24" s="45"/>
+      <c r="BE24" s="45"/>
       <c r="BU24" s="30"/>
       <c r="BV24" s="30"/>
       <c r="BW24" s="30"/>
@@ -11297,18 +12829,18 @@
       <c r="CQ24" s="30"/>
     </row>
     <row r="28" spans="3:97" x14ac:dyDescent="0.15">
-      <c r="AI28" s="48" t="s">
+      <c r="AI28" s="53" t="s">
         <v>178</v>
       </c>
-      <c r="AJ28" s="42"/>
-      <c r="AK28" s="42"/>
-      <c r="AL28" s="42"/>
+      <c r="AJ28" s="44"/>
+      <c r="AK28" s="44"/>
+      <c r="AL28" s="44"/>
     </row>
     <row r="29" spans="3:97" x14ac:dyDescent="0.15">
-      <c r="AI29" s="42"/>
-      <c r="AJ29" s="42"/>
-      <c r="AK29" s="42"/>
-      <c r="AL29" s="42"/>
+      <c r="AI29" s="44"/>
+      <c r="AJ29" s="44"/>
+      <c r="AK29" s="44"/>
+      <c r="AL29" s="44"/>
       <c r="AM29" s="29"/>
       <c r="AN29" s="29"/>
       <c r="AO29" s="29"/>
@@ -11319,10 +12851,10 @@
       <c r="AT29" s="29"/>
     </row>
     <row r="30" spans="3:97" x14ac:dyDescent="0.15">
-      <c r="AI30" s="42"/>
-      <c r="AJ30" s="42"/>
-      <c r="AK30" s="42"/>
-      <c r="AL30" s="42"/>
+      <c r="AI30" s="44"/>
+      <c r="AJ30" s="44"/>
+      <c r="AK30" s="44"/>
+      <c r="AL30" s="44"/>
       <c r="AM30" s="29"/>
       <c r="AN30" s="29"/>
       <c r="AO30" s="29"/>
@@ -11333,26 +12865,26 @@
       <c r="AT30" s="29"/>
     </row>
     <row r="31" spans="3:97" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D31" s="44" t="s">
+      <c r="D31" s="45" t="s">
         <v>154</v>
       </c>
-      <c r="E31" s="45"/>
+      <c r="E31" s="50"/>
       <c r="F31" s="46"/>
       <c r="G31" s="46"/>
       <c r="H31" s="46"/>
       <c r="I31" s="46"/>
-      <c r="U31" s="44" t="s">
+      <c r="U31" s="45" t="s">
         <v>172</v>
       </c>
-      <c r="V31" s="44"/>
-      <c r="W31" s="44"/>
-      <c r="X31" s="44"/>
-      <c r="Y31" s="44"/>
-      <c r="Z31" s="44"/>
-      <c r="AI31" s="42"/>
-      <c r="AJ31" s="42"/>
-      <c r="AK31" s="42"/>
-      <c r="AL31" s="42"/>
+      <c r="V31" s="45"/>
+      <c r="W31" s="45"/>
+      <c r="X31" s="45"/>
+      <c r="Y31" s="45"/>
+      <c r="Z31" s="45"/>
+      <c r="AI31" s="44"/>
+      <c r="AJ31" s="44"/>
+      <c r="AK31" s="44"/>
+      <c r="AL31" s="44"/>
       <c r="AM31" s="30"/>
       <c r="AN31" s="30"/>
       <c r="AO31" s="30"/>
@@ -11361,42 +12893,42 @@
       <c r="AR31" s="29"/>
       <c r="AS31" s="29"/>
       <c r="AT31" s="29"/>
-      <c r="AZ31" s="44" t="s">
+      <c r="AZ31" s="45" t="s">
         <v>173</v>
       </c>
-      <c r="BA31" s="44"/>
-      <c r="BB31" s="44"/>
-      <c r="BC31" s="44"/>
-      <c r="BD31" s="44"/>
-      <c r="BE31" s="44"/>
+      <c r="BA31" s="45"/>
+      <c r="BB31" s="45"/>
+      <c r="BC31" s="45"/>
+      <c r="BD31" s="45"/>
+      <c r="BE31" s="45"/>
       <c r="BU31" s="30"/>
       <c r="BV31" s="30"/>
       <c r="BW31" s="30"/>
       <c r="BX31" s="30"/>
       <c r="BY31" s="30"/>
       <c r="BZ31" s="30"/>
-      <c r="CL31" s="44" t="s">
+      <c r="CL31" s="45" t="s">
         <v>173</v>
       </c>
-      <c r="CM31" s="44"/>
-      <c r="CN31" s="44"/>
-      <c r="CO31" s="44"/>
-      <c r="CP31" s="44"/>
-      <c r="CQ31" s="44"/>
+      <c r="CM31" s="45"/>
+      <c r="CN31" s="45"/>
+      <c r="CO31" s="45"/>
+      <c r="CP31" s="45"/>
+      <c r="CQ31" s="45"/>
     </row>
     <row r="32" spans="3:97" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D32" s="45"/>
-      <c r="E32" s="45"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="50"/>
       <c r="F32" s="46"/>
       <c r="G32" s="46"/>
       <c r="H32" s="46"/>
       <c r="I32" s="46"/>
-      <c r="U32" s="44"/>
-      <c r="V32" s="44"/>
-      <c r="W32" s="44"/>
-      <c r="X32" s="44"/>
-      <c r="Y32" s="44"/>
-      <c r="Z32" s="44"/>
+      <c r="U32" s="45"/>
+      <c r="V32" s="45"/>
+      <c r="W32" s="45"/>
+      <c r="X32" s="45"/>
+      <c r="Y32" s="45"/>
+      <c r="Z32" s="45"/>
       <c r="AJ32" s="29"/>
       <c r="AK32" s="30"/>
       <c r="AL32" s="30"/>
@@ -11408,24 +12940,24 @@
       <c r="AR32" s="29"/>
       <c r="AS32" s="29"/>
       <c r="AT32" s="29"/>
-      <c r="AZ32" s="44"/>
-      <c r="BA32" s="44"/>
-      <c r="BB32" s="44"/>
-      <c r="BC32" s="44"/>
-      <c r="BD32" s="44"/>
-      <c r="BE32" s="44"/>
+      <c r="AZ32" s="45"/>
+      <c r="BA32" s="45"/>
+      <c r="BB32" s="45"/>
+      <c r="BC32" s="45"/>
+      <c r="BD32" s="45"/>
+      <c r="BE32" s="45"/>
       <c r="BU32" s="30"/>
       <c r="BV32" s="30"/>
       <c r="BW32" s="30"/>
       <c r="BX32" s="30"/>
       <c r="BY32" s="30"/>
       <c r="BZ32" s="30"/>
-      <c r="CL32" s="44"/>
-      <c r="CM32" s="44"/>
-      <c r="CN32" s="44"/>
-      <c r="CO32" s="44"/>
-      <c r="CP32" s="44"/>
-      <c r="CQ32" s="44"/>
+      <c r="CL32" s="45"/>
+      <c r="CM32" s="45"/>
+      <c r="CN32" s="45"/>
+      <c r="CO32" s="45"/>
+      <c r="CP32" s="45"/>
+      <c r="CQ32" s="45"/>
     </row>
     <row r="33" spans="4:99" x14ac:dyDescent="0.15">
       <c r="AJ33" s="29"/>
@@ -11441,14 +12973,14 @@
       <c r="AT33" s="29"/>
     </row>
     <row r="34" spans="4:99" x14ac:dyDescent="0.15">
-      <c r="AH34" s="53" t="s">
+      <c r="AH34" s="55" t="s">
         <v>183</v>
       </c>
-      <c r="AI34" s="42"/>
-      <c r="AJ34" s="42"/>
-      <c r="AK34" s="42"/>
-      <c r="AL34" s="42"/>
-      <c r="AM34" s="42"/>
+      <c r="AI34" s="44"/>
+      <c r="AJ34" s="44"/>
+      <c r="AK34" s="44"/>
+      <c r="AL34" s="44"/>
+      <c r="AM34" s="44"/>
       <c r="AN34" s="29"/>
       <c r="AO34" s="29"/>
       <c r="AP34" s="29"/>
@@ -11458,12 +12990,12 @@
       <c r="AT34" s="29"/>
     </row>
     <row r="35" spans="4:99" x14ac:dyDescent="0.15">
-      <c r="AH35" s="42"/>
-      <c r="AI35" s="42"/>
-      <c r="AJ35" s="42"/>
-      <c r="AK35" s="42"/>
-      <c r="AL35" s="42"/>
-      <c r="AM35" s="42"/>
+      <c r="AH35" s="44"/>
+      <c r="AI35" s="44"/>
+      <c r="AJ35" s="44"/>
+      <c r="AK35" s="44"/>
+      <c r="AL35" s="44"/>
+      <c r="AM35" s="44"/>
       <c r="AN35" s="29"/>
       <c r="AO35" s="29"/>
       <c r="AP35" s="29"/>
@@ -11471,22 +13003,22 @@
       <c r="AR35" s="29"/>
       <c r="AS35" s="29"/>
       <c r="AT35" s="29"/>
-      <c r="BU35" s="43" t="s">
+      <c r="BU35" s="48" t="s">
         <v>191</v>
       </c>
-      <c r="BV35" s="43"/>
-      <c r="BW35" s="43"/>
-      <c r="BX35" s="43"/>
-      <c r="BY35" s="43"/>
-      <c r="BZ35" s="43"/>
+      <c r="BV35" s="48"/>
+      <c r="BW35" s="48"/>
+      <c r="BX35" s="48"/>
+      <c r="BY35" s="48"/>
+      <c r="BZ35" s="48"/>
     </row>
     <row r="36" spans="4:99" x14ac:dyDescent="0.15">
-      <c r="AH36" s="42"/>
-      <c r="AI36" s="42"/>
-      <c r="AJ36" s="42"/>
-      <c r="AK36" s="42"/>
-      <c r="AL36" s="42"/>
-      <c r="AM36" s="42"/>
+      <c r="AH36" s="44"/>
+      <c r="AI36" s="44"/>
+      <c r="AJ36" s="44"/>
+      <c r="AK36" s="44"/>
+      <c r="AL36" s="44"/>
+      <c r="AM36" s="44"/>
       <c r="AN36" s="29"/>
       <c r="AO36" s="29"/>
       <c r="AP36" s="29"/>
@@ -11494,20 +13026,20 @@
       <c r="AR36" s="29"/>
       <c r="AS36" s="29"/>
       <c r="AT36" s="29"/>
-      <c r="BU36" s="43"/>
-      <c r="BV36" s="43"/>
-      <c r="BW36" s="43"/>
-      <c r="BX36" s="43"/>
-      <c r="BY36" s="43"/>
-      <c r="BZ36" s="43"/>
+      <c r="BU36" s="48"/>
+      <c r="BV36" s="48"/>
+      <c r="BW36" s="48"/>
+      <c r="BX36" s="48"/>
+      <c r="BY36" s="48"/>
+      <c r="BZ36" s="48"/>
     </row>
     <row r="37" spans="4:99" x14ac:dyDescent="0.15">
-      <c r="AH37" s="42"/>
-      <c r="AI37" s="42"/>
-      <c r="AJ37" s="42"/>
-      <c r="AK37" s="42"/>
-      <c r="AL37" s="42"/>
-      <c r="AM37" s="42"/>
+      <c r="AH37" s="44"/>
+      <c r="AI37" s="44"/>
+      <c r="AJ37" s="44"/>
+      <c r="AK37" s="44"/>
+      <c r="AL37" s="44"/>
+      <c r="AM37" s="44"/>
       <c r="AN37" s="29"/>
       <c r="AO37" s="29"/>
       <c r="AP37" s="29"/>
@@ -11517,22 +13049,22 @@
       <c r="AT37" s="29"/>
     </row>
     <row r="38" spans="4:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D38" s="44" t="s">
+      <c r="D38" s="45" t="s">
         <v>159</v>
       </c>
-      <c r="E38" s="45"/>
+      <c r="E38" s="50"/>
       <c r="F38" s="46"/>
       <c r="G38" s="46"/>
       <c r="H38" s="46"/>
       <c r="I38" s="46"/>
       <c r="AB38" s="30"/>
       <c r="AC38" s="30"/>
-      <c r="AI38" s="43" t="s">
+      <c r="AI38" s="48" t="s">
         <v>179</v>
       </c>
-      <c r="AJ38" s="42"/>
-      <c r="AK38" s="42"/>
-      <c r="AL38" s="42"/>
+      <c r="AJ38" s="44"/>
+      <c r="AK38" s="44"/>
+      <c r="AL38" s="44"/>
       <c r="AM38" s="29"/>
       <c r="AN38" s="29"/>
       <c r="AO38" s="29"/>
@@ -11542,7 +13074,7 @@
       <c r="AS38" s="29"/>
       <c r="AT38" s="29"/>
       <c r="AU38" s="29"/>
-      <c r="AZ38" s="44" t="s">
+      <c r="AZ38" s="45" t="s">
         <v>174</v>
       </c>
       <c r="BA38" s="46"/>
@@ -11554,12 +13086,12 @@
       <c r="BG38" s="46"/>
       <c r="BH38" s="46"/>
       <c r="BI38" s="46"/>
-      <c r="BV38" s="47" t="s">
+      <c r="BV38" s="49" t="s">
         <v>192</v>
       </c>
       <c r="BW38" s="46"/>
       <c r="BX38" s="46"/>
-      <c r="CL38" s="44" t="s">
+      <c r="CL38" s="45" t="s">
         <v>174</v>
       </c>
       <c r="CM38" s="46"/>
@@ -11573,18 +13105,18 @@
       <c r="CU38" s="46"/>
     </row>
     <row r="39" spans="4:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D39" s="45"/>
-      <c r="E39" s="45"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
       <c r="F39" s="46"/>
       <c r="G39" s="46"/>
       <c r="H39" s="46"/>
       <c r="I39" s="46"/>
       <c r="AB39" s="30"/>
       <c r="AC39" s="30"/>
-      <c r="AI39" s="42"/>
-      <c r="AJ39" s="42"/>
-      <c r="AK39" s="42"/>
-      <c r="AL39" s="42"/>
+      <c r="AI39" s="44"/>
+      <c r="AJ39" s="44"/>
+      <c r="AK39" s="44"/>
+      <c r="AL39" s="44"/>
       <c r="AM39" s="29"/>
       <c r="AN39" s="29"/>
       <c r="AO39" s="29"/>
@@ -11619,10 +13151,10 @@
       <c r="CU39" s="46"/>
     </row>
     <row r="40" spans="4:99" x14ac:dyDescent="0.15">
-      <c r="AI40" s="42"/>
-      <c r="AJ40" s="42"/>
-      <c r="AK40" s="42"/>
-      <c r="AL40" s="42"/>
+      <c r="AI40" s="44"/>
+      <c r="AJ40" s="44"/>
+      <c r="AK40" s="44"/>
+      <c r="AL40" s="44"/>
       <c r="AM40" s="29"/>
       <c r="AN40" s="29"/>
       <c r="AO40" s="29"/>
@@ -11633,14 +13165,14 @@
       <c r="AT40" s="29"/>
     </row>
     <row r="41" spans="4:99" x14ac:dyDescent="0.15">
-      <c r="AH41" s="50" t="s">
+      <c r="AH41" s="56" t="s">
         <v>180</v>
       </c>
-      <c r="AI41" s="42"/>
-      <c r="AJ41" s="42"/>
-      <c r="AK41" s="42"/>
-      <c r="AL41" s="42"/>
-      <c r="AM41" s="42"/>
+      <c r="AI41" s="44"/>
+      <c r="AJ41" s="44"/>
+      <c r="AK41" s="44"/>
+      <c r="AL41" s="44"/>
+      <c r="AM41" s="44"/>
       <c r="AN41" s="29"/>
       <c r="AO41" s="29"/>
       <c r="AP41" s="29"/>
@@ -11648,32 +13180,32 @@
       <c r="AR41" s="29"/>
       <c r="AS41" s="29"/>
       <c r="AT41" s="29"/>
-      <c r="BU41" s="48" t="s">
+      <c r="BU41" s="53" t="s">
         <v>193</v>
       </c>
-      <c r="BV41" s="42"/>
-      <c r="BW41" s="42"/>
-      <c r="BX41" s="42"/>
-      <c r="BY41" s="42"/>
-      <c r="BZ41" s="42"/>
+      <c r="BV41" s="44"/>
+      <c r="BW41" s="44"/>
+      <c r="BX41" s="44"/>
+      <c r="BY41" s="44"/>
+      <c r="BZ41" s="44"/>
     </row>
     <row r="42" spans="4:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="M42" s="43" t="s">
+      <c r="M42" s="48" t="s">
         <v>203</v>
       </c>
-      <c r="N42" s="42"/>
-      <c r="O42" s="42"/>
-      <c r="Z42" s="43" t="s">
+      <c r="N42" s="44"/>
+      <c r="O42" s="44"/>
+      <c r="Z42" s="48" t="s">
         <v>202</v>
       </c>
-      <c r="AA42" s="42"/>
-      <c r="AB42" s="42"/>
-      <c r="AH42" s="42"/>
-      <c r="AI42" s="42"/>
-      <c r="AJ42" s="42"/>
-      <c r="AK42" s="42"/>
-      <c r="AL42" s="42"/>
-      <c r="AM42" s="42"/>
+      <c r="AA42" s="44"/>
+      <c r="AB42" s="44"/>
+      <c r="AH42" s="44"/>
+      <c r="AI42" s="44"/>
+      <c r="AJ42" s="44"/>
+      <c r="AK42" s="44"/>
+      <c r="AL42" s="44"/>
+      <c r="AM42" s="44"/>
       <c r="AN42" s="29"/>
       <c r="AO42" s="29"/>
       <c r="AP42" s="29"/>
@@ -11681,30 +13213,30 @@
       <c r="AR42" s="29"/>
       <c r="AS42" s="29"/>
       <c r="AT42" s="29"/>
-      <c r="BU42" s="42"/>
-      <c r="BV42" s="42"/>
-      <c r="BW42" s="42"/>
-      <c r="BX42" s="42"/>
-      <c r="BY42" s="42"/>
-      <c r="BZ42" s="42"/>
+      <c r="BU42" s="44"/>
+      <c r="BV42" s="44"/>
+      <c r="BW42" s="44"/>
+      <c r="BX42" s="44"/>
+      <c r="BY42" s="44"/>
+      <c r="BZ42" s="44"/>
       <c r="CA42" s="29"/>
       <c r="CB42" s="29"/>
       <c r="CG42" s="29"/>
       <c r="CH42" s="29"/>
     </row>
     <row r="43" spans="4:99" x14ac:dyDescent="0.15">
-      <c r="M43" s="42"/>
-      <c r="N43" s="42"/>
-      <c r="O43" s="42"/>
-      <c r="Z43" s="42"/>
-      <c r="AA43" s="42"/>
-      <c r="AB43" s="42"/>
-      <c r="AH43" s="42"/>
-      <c r="AI43" s="42"/>
-      <c r="AJ43" s="42"/>
-      <c r="AK43" s="42"/>
-      <c r="AL43" s="42"/>
-      <c r="AM43" s="42"/>
+      <c r="M43" s="44"/>
+      <c r="N43" s="44"/>
+      <c r="O43" s="44"/>
+      <c r="Z43" s="44"/>
+      <c r="AA43" s="44"/>
+      <c r="AB43" s="44"/>
+      <c r="AH43" s="44"/>
+      <c r="AI43" s="44"/>
+      <c r="AJ43" s="44"/>
+      <c r="AK43" s="44"/>
+      <c r="AL43" s="44"/>
+      <c r="AM43" s="44"/>
       <c r="AN43" s="29"/>
       <c r="AO43" s="29"/>
       <c r="AP43" s="29"/>
@@ -11712,24 +13244,24 @@
       <c r="AR43" s="29"/>
       <c r="AS43" s="29"/>
       <c r="AT43" s="29"/>
-      <c r="BU43" s="42"/>
-      <c r="BV43" s="42"/>
-      <c r="BW43" s="42"/>
-      <c r="BX43" s="42"/>
-      <c r="BY43" s="42"/>
-      <c r="BZ43" s="42"/>
+      <c r="BU43" s="44"/>
+      <c r="BV43" s="44"/>
+      <c r="BW43" s="44"/>
+      <c r="BX43" s="44"/>
+      <c r="BY43" s="44"/>
+      <c r="BZ43" s="44"/>
       <c r="CA43" s="29"/>
       <c r="CB43" s="29"/>
       <c r="CG43" s="29"/>
       <c r="CH43" s="29"/>
     </row>
     <row r="44" spans="4:99" x14ac:dyDescent="0.15">
-      <c r="AH44" s="42"/>
-      <c r="AI44" s="42"/>
-      <c r="AJ44" s="42"/>
-      <c r="AK44" s="42"/>
-      <c r="AL44" s="42"/>
-      <c r="AM44" s="42"/>
+      <c r="AH44" s="44"/>
+      <c r="AI44" s="44"/>
+      <c r="AJ44" s="44"/>
+      <c r="AK44" s="44"/>
+      <c r="AL44" s="44"/>
+      <c r="AM44" s="44"/>
       <c r="AN44" s="29"/>
       <c r="AO44" s="29"/>
       <c r="AP44" s="29"/>
@@ -11737,15 +13269,15 @@
       <c r="AR44" s="29"/>
       <c r="AS44" s="29"/>
       <c r="AT44" s="29"/>
-      <c r="BU44" s="42"/>
-      <c r="BV44" s="42"/>
-      <c r="BW44" s="42"/>
-      <c r="BX44" s="42"/>
-      <c r="BY44" s="42"/>
-      <c r="BZ44" s="42"/>
+      <c r="BU44" s="44"/>
+      <c r="BV44" s="44"/>
+      <c r="BW44" s="44"/>
+      <c r="BX44" s="44"/>
+      <c r="BY44" s="44"/>
+      <c r="BZ44" s="44"/>
     </row>
     <row r="45" spans="4:99" x14ac:dyDescent="0.15">
-      <c r="R45" s="43" t="s">
+      <c r="R45" s="48" t="s">
         <v>167</v>
       </c>
       <c r="S45" s="46"/>
@@ -11766,10 +13298,10 @@
       <c r="AT45" s="29"/>
     </row>
     <row r="46" spans="4:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D46" s="44" t="s">
+      <c r="D46" s="45" t="s">
         <v>156</v>
       </c>
-      <c r="E46" s="45"/>
+      <c r="E46" s="50"/>
       <c r="F46" s="46"/>
       <c r="G46" s="46"/>
       <c r="H46" s="46"/>
@@ -11797,32 +13329,32 @@
       <c r="AR46" s="29"/>
       <c r="AS46" s="29"/>
       <c r="AT46" s="29"/>
-      <c r="AZ46" s="44" t="s">
+      <c r="AZ46" s="45" t="s">
         <v>156</v>
       </c>
-      <c r="BA46" s="45"/>
+      <c r="BA46" s="50"/>
       <c r="BB46" s="46"/>
       <c r="BC46" s="46"/>
       <c r="BD46" s="46"/>
       <c r="BE46" s="46"/>
-      <c r="BW46" s="54" t="s">
+      <c r="BW46" s="52" t="s">
         <v>194</v>
       </c>
-      <c r="BX46" s="42"/>
-      <c r="BY46" s="42"/>
-      <c r="BZ46" s="42"/>
-      <c r="CL46" s="44" t="s">
+      <c r="BX46" s="44"/>
+      <c r="BY46" s="44"/>
+      <c r="BZ46" s="44"/>
+      <c r="CL46" s="45" t="s">
         <v>156</v>
       </c>
-      <c r="CM46" s="45"/>
+      <c r="CM46" s="50"/>
       <c r="CN46" s="46"/>
       <c r="CO46" s="46"/>
       <c r="CP46" s="46"/>
       <c r="CQ46" s="46"/>
     </row>
     <row r="47" spans="4:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D47" s="45"/>
-      <c r="E47" s="45"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="50"/>
       <c r="F47" s="46"/>
       <c r="G47" s="46"/>
       <c r="H47" s="46"/>
@@ -11850,18 +13382,18 @@
       <c r="AR47" s="29"/>
       <c r="AS47" s="29"/>
       <c r="AT47" s="29"/>
-      <c r="AZ47" s="45"/>
-      <c r="BA47" s="45"/>
+      <c r="AZ47" s="50"/>
+      <c r="BA47" s="50"/>
       <c r="BB47" s="46"/>
       <c r="BC47" s="46"/>
       <c r="BD47" s="46"/>
       <c r="BE47" s="46"/>
-      <c r="BW47" s="42"/>
-      <c r="BX47" s="42"/>
-      <c r="BY47" s="42"/>
-      <c r="BZ47" s="42"/>
-      <c r="CL47" s="45"/>
-      <c r="CM47" s="45"/>
+      <c r="BW47" s="44"/>
+      <c r="BX47" s="44"/>
+      <c r="BY47" s="44"/>
+      <c r="BZ47" s="44"/>
+      <c r="CL47" s="50"/>
+      <c r="CM47" s="50"/>
       <c r="CN47" s="46"/>
       <c r="CO47" s="46"/>
       <c r="CP47" s="46"/>
@@ -11887,14 +13419,14 @@
       <c r="AT48" s="29"/>
     </row>
     <row r="49" spans="4:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="AH49" s="51" t="s">
+      <c r="AH49" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="AI49" s="42"/>
-      <c r="AJ49" s="42"/>
-      <c r="AK49" s="42"/>
-      <c r="AL49" s="42"/>
-      <c r="AM49" s="42"/>
+      <c r="AI49" s="44"/>
+      <c r="AJ49" s="44"/>
+      <c r="AK49" s="44"/>
+      <c r="AL49" s="44"/>
+      <c r="AM49" s="44"/>
       <c r="AN49" s="29"/>
       <c r="AO49" s="29"/>
       <c r="AP49" s="29"/>
@@ -11904,12 +13436,12 @@
       <c r="AT49" s="29"/>
     </row>
     <row r="50" spans="4:98" x14ac:dyDescent="0.15">
-      <c r="AH50" s="42"/>
-      <c r="AI50" s="42"/>
-      <c r="AJ50" s="42"/>
-      <c r="AK50" s="42"/>
-      <c r="AL50" s="42"/>
-      <c r="AM50" s="42"/>
+      <c r="AH50" s="44"/>
+      <c r="AI50" s="44"/>
+      <c r="AJ50" s="44"/>
+      <c r="AK50" s="44"/>
+      <c r="AL50" s="44"/>
+      <c r="AM50" s="44"/>
       <c r="AN50" s="29"/>
       <c r="AO50" s="29"/>
       <c r="AP50" s="29"/>
@@ -11917,23 +13449,23 @@
       <c r="AR50" s="29"/>
       <c r="AS50" s="29"/>
       <c r="AT50" s="29"/>
-      <c r="BU50" s="43" t="s">
+      <c r="BU50" s="48" t="s">
         <v>196</v>
       </c>
-      <c r="BV50" s="42"/>
-      <c r="BW50" s="42"/>
-      <c r="BX50" s="42"/>
-      <c r="BY50" s="42"/>
-      <c r="BZ50" s="42"/>
-      <c r="CA50" s="42"/>
+      <c r="BV50" s="44"/>
+      <c r="BW50" s="44"/>
+      <c r="BX50" s="44"/>
+      <c r="BY50" s="44"/>
+      <c r="BZ50" s="44"/>
+      <c r="CA50" s="44"/>
     </row>
     <row r="51" spans="4:98" x14ac:dyDescent="0.15">
-      <c r="AH51" s="42"/>
-      <c r="AI51" s="42"/>
-      <c r="AJ51" s="42"/>
-      <c r="AK51" s="42"/>
-      <c r="AL51" s="42"/>
-      <c r="AM51" s="42"/>
+      <c r="AH51" s="44"/>
+      <c r="AI51" s="44"/>
+      <c r="AJ51" s="44"/>
+      <c r="AK51" s="44"/>
+      <c r="AL51" s="44"/>
+      <c r="AM51" s="44"/>
       <c r="AN51" s="29"/>
       <c r="AO51" s="29"/>
       <c r="AP51" s="29"/>
@@ -11941,29 +13473,29 @@
       <c r="AR51" s="29"/>
       <c r="AS51" s="29"/>
       <c r="AT51" s="29"/>
-      <c r="BU51" s="42"/>
-      <c r="BV51" s="42"/>
-      <c r="BW51" s="42"/>
-      <c r="BX51" s="42"/>
-      <c r="BY51" s="42"/>
-      <c r="BZ51" s="42"/>
-      <c r="CA51" s="42"/>
+      <c r="BU51" s="44"/>
+      <c r="BV51" s="44"/>
+      <c r="BW51" s="44"/>
+      <c r="BX51" s="44"/>
+      <c r="BY51" s="44"/>
+      <c r="BZ51" s="44"/>
+      <c r="CA51" s="44"/>
     </row>
     <row r="52" spans="4:98" x14ac:dyDescent="0.15">
-      <c r="R52" s="43" t="s">
+      <c r="R52" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="S52" s="43"/>
-      <c r="T52" s="43"/>
-      <c r="U52" s="43"/>
-      <c r="V52" s="43"/>
-      <c r="W52" s="43"/>
-      <c r="AH52" s="42"/>
-      <c r="AI52" s="42"/>
-      <c r="AJ52" s="42"/>
-      <c r="AK52" s="42"/>
-      <c r="AL52" s="42"/>
-      <c r="AM52" s="42"/>
+      <c r="S52" s="48"/>
+      <c r="T52" s="48"/>
+      <c r="U52" s="48"/>
+      <c r="V52" s="48"/>
+      <c r="W52" s="48"/>
+      <c r="AH52" s="44"/>
+      <c r="AI52" s="44"/>
+      <c r="AJ52" s="44"/>
+      <c r="AK52" s="44"/>
+      <c r="AL52" s="44"/>
+      <c r="AM52" s="44"/>
       <c r="AN52" s="29"/>
       <c r="AO52" s="29"/>
       <c r="AP52" s="29"/>
@@ -11973,22 +13505,22 @@
       <c r="AT52" s="29"/>
     </row>
     <row r="53" spans="4:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D53" s="44" t="s">
+      <c r="D53" s="45" t="s">
         <v>155</v>
       </c>
-      <c r="E53" s="44"/>
-      <c r="F53" s="44"/>
-      <c r="G53" s="44"/>
-      <c r="H53" s="44"/>
-      <c r="I53" s="44"/>
+      <c r="E53" s="45"/>
+      <c r="F53" s="45"/>
+      <c r="G53" s="45"/>
+      <c r="H53" s="45"/>
+      <c r="I53" s="45"/>
       <c r="P53" s="30"/>
       <c r="Q53" s="30"/>
-      <c r="R53" s="43"/>
-      <c r="S53" s="43"/>
-      <c r="T53" s="43"/>
-      <c r="U53" s="43"/>
-      <c r="V53" s="43"/>
-      <c r="W53" s="43"/>
+      <c r="R53" s="48"/>
+      <c r="S53" s="48"/>
+      <c r="T53" s="48"/>
+      <c r="U53" s="48"/>
+      <c r="V53" s="48"/>
+      <c r="W53" s="48"/>
       <c r="AJ53" s="29"/>
       <c r="AK53" s="30"/>
       <c r="AL53" s="30"/>
@@ -12000,19 +13532,19 @@
       <c r="AR53" s="29"/>
       <c r="AS53" s="29"/>
       <c r="AT53" s="29"/>
-      <c r="AZ53" s="44" t="s">
+      <c r="AZ53" s="45" t="s">
         <v>175</v>
       </c>
-      <c r="BA53" s="44"/>
-      <c r="BB53" s="44"/>
-      <c r="BC53" s="44"/>
-      <c r="BD53" s="44"/>
-      <c r="BE53" s="44"/>
-      <c r="BV53" s="52" t="s">
+      <c r="BA53" s="45"/>
+      <c r="BB53" s="45"/>
+      <c r="BC53" s="45"/>
+      <c r="BD53" s="45"/>
+      <c r="BE53" s="45"/>
+      <c r="BV53" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="BW53" s="42"/>
-      <c r="BX53" s="42"/>
+      <c r="BW53" s="44"/>
+      <c r="BX53" s="44"/>
       <c r="CL53" s="30"/>
       <c r="CM53" s="30"/>
       <c r="CN53" s="30"/>
@@ -12024,20 +13556,20 @@
       <c r="CT53" s="29"/>
     </row>
     <row r="54" spans="4:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D54" s="44"/>
-      <c r="E54" s="44"/>
-      <c r="F54" s="44"/>
-      <c r="G54" s="44"/>
-      <c r="H54" s="44"/>
-      <c r="I54" s="44"/>
+      <c r="D54" s="45"/>
+      <c r="E54" s="45"/>
+      <c r="F54" s="45"/>
+      <c r="G54" s="45"/>
+      <c r="H54" s="45"/>
+      <c r="I54" s="45"/>
       <c r="P54" s="30"/>
       <c r="Q54" s="30"/>
-      <c r="R54" s="42"/>
-      <c r="S54" s="42"/>
-      <c r="T54" s="42"/>
-      <c r="U54" s="42"/>
-      <c r="V54" s="42"/>
-      <c r="W54" s="42"/>
+      <c r="R54" s="44"/>
+      <c r="S54" s="44"/>
+      <c r="T54" s="44"/>
+      <c r="U54" s="44"/>
+      <c r="V54" s="44"/>
+      <c r="W54" s="44"/>
       <c r="AJ54" s="29"/>
       <c r="AK54" s="30"/>
       <c r="AL54" s="30"/>
@@ -12049,15 +13581,15 @@
       <c r="AR54" s="29"/>
       <c r="AS54" s="29"/>
       <c r="AT54" s="29"/>
-      <c r="AZ54" s="44"/>
-      <c r="BA54" s="44"/>
-      <c r="BB54" s="44"/>
-      <c r="BC54" s="44"/>
-      <c r="BD54" s="44"/>
-      <c r="BE54" s="44"/>
-      <c r="BV54" s="42"/>
-      <c r="BW54" s="42"/>
-      <c r="BX54" s="42"/>
+      <c r="AZ54" s="45"/>
+      <c r="BA54" s="45"/>
+      <c r="BB54" s="45"/>
+      <c r="BC54" s="45"/>
+      <c r="BD54" s="45"/>
+      <c r="BE54" s="45"/>
+      <c r="BV54" s="44"/>
+      <c r="BW54" s="44"/>
+      <c r="BX54" s="44"/>
       <c r="CL54" s="30"/>
       <c r="CM54" s="30"/>
       <c r="CN54" s="30"/>
@@ -12069,12 +13601,12 @@
       <c r="CT54" s="29"/>
     </row>
     <row r="55" spans="4:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="R55" s="42"/>
-      <c r="S55" s="42"/>
-      <c r="T55" s="42"/>
-      <c r="U55" s="42"/>
-      <c r="V55" s="42"/>
-      <c r="W55" s="42"/>
+      <c r="R55" s="44"/>
+      <c r="S55" s="44"/>
+      <c r="T55" s="44"/>
+      <c r="U55" s="44"/>
+      <c r="V55" s="44"/>
+      <c r="W55" s="44"/>
       <c r="AJ55" s="29"/>
       <c r="AK55" s="29"/>
       <c r="AL55" s="29"/>
@@ -12097,14 +13629,14 @@
       <c r="CT55" s="29"/>
     </row>
     <row r="56" spans="4:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="AH56" s="52" t="s">
+      <c r="AH56" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="AI56" s="42"/>
-      <c r="AJ56" s="42"/>
-      <c r="AK56" s="42"/>
-      <c r="AL56" s="42"/>
-      <c r="AM56" s="42"/>
+      <c r="AI56" s="44"/>
+      <c r="AJ56" s="44"/>
+      <c r="AK56" s="44"/>
+      <c r="AL56" s="44"/>
+      <c r="AM56" s="44"/>
       <c r="AN56" s="29"/>
       <c r="AO56" s="29"/>
       <c r="AP56" s="29"/>
@@ -12123,12 +13655,12 @@
       <c r="CT56" s="29"/>
     </row>
     <row r="57" spans="4:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="AH57" s="42"/>
-      <c r="AI57" s="42"/>
-      <c r="AJ57" s="42"/>
-      <c r="AK57" s="42"/>
-      <c r="AL57" s="42"/>
-      <c r="AM57" s="42"/>
+      <c r="AH57" s="44"/>
+      <c r="AI57" s="44"/>
+      <c r="AJ57" s="44"/>
+      <c r="AK57" s="44"/>
+      <c r="AL57" s="44"/>
+      <c r="AM57" s="44"/>
       <c r="AN57" s="29"/>
       <c r="AO57" s="29"/>
       <c r="AP57" s="29"/>
@@ -12136,14 +13668,14 @@
       <c r="AR57" s="29"/>
       <c r="AS57" s="29"/>
       <c r="AT57" s="29"/>
-      <c r="BU57" s="43" t="s">
+      <c r="BU57" s="48" t="s">
         <v>197</v>
       </c>
-      <c r="BV57" s="43"/>
-      <c r="BW57" s="43"/>
-      <c r="BX57" s="43"/>
-      <c r="BY57" s="43"/>
-      <c r="BZ57" s="43"/>
+      <c r="BV57" s="48"/>
+      <c r="BW57" s="48"/>
+      <c r="BX57" s="48"/>
+      <c r="BY57" s="48"/>
+      <c r="BZ57" s="48"/>
       <c r="CL57" s="29"/>
       <c r="CM57" s="29"/>
       <c r="CN57" s="29"/>
@@ -12155,18 +13687,18 @@
       <c r="CT57" s="29"/>
     </row>
     <row r="58" spans="4:98" x14ac:dyDescent="0.15">
-      <c r="S58" s="52" t="s">
+      <c r="S58" s="54" t="s">
         <v>168</v>
       </c>
-      <c r="T58" s="42"/>
-      <c r="U58" s="42"/>
-      <c r="V58" s="42"/>
-      <c r="AH58" s="42"/>
-      <c r="AI58" s="42"/>
-      <c r="AJ58" s="42"/>
-      <c r="AK58" s="42"/>
-      <c r="AL58" s="42"/>
-      <c r="AM58" s="42"/>
+      <c r="T58" s="44"/>
+      <c r="U58" s="44"/>
+      <c r="V58" s="44"/>
+      <c r="AH58" s="44"/>
+      <c r="AI58" s="44"/>
+      <c r="AJ58" s="44"/>
+      <c r="AK58" s="44"/>
+      <c r="AL58" s="44"/>
+      <c r="AM58" s="44"/>
       <c r="AN58" s="29"/>
       <c r="AO58" s="29"/>
       <c r="AP58" s="29"/>
@@ -12174,12 +13706,12 @@
       <c r="AR58" s="29"/>
       <c r="AS58" s="29"/>
       <c r="AT58" s="29"/>
-      <c r="BU58" s="43"/>
-      <c r="BV58" s="43"/>
-      <c r="BW58" s="43"/>
-      <c r="BX58" s="43"/>
-      <c r="BY58" s="43"/>
-      <c r="BZ58" s="43"/>
+      <c r="BU58" s="48"/>
+      <c r="BV58" s="48"/>
+      <c r="BW58" s="48"/>
+      <c r="BX58" s="48"/>
+      <c r="BY58" s="48"/>
+      <c r="BZ58" s="48"/>
       <c r="CL58" s="29"/>
       <c r="CM58" s="29"/>
       <c r="CN58" s="29"/>
@@ -12191,32 +13723,32 @@
       <c r="CT58" s="29"/>
     </row>
     <row r="59" spans="4:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E59" s="44" t="s">
+      <c r="E59" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="F59" s="44"/>
-      <c r="G59" s="44"/>
-      <c r="H59" s="44"/>
-      <c r="I59" s="44"/>
-      <c r="J59" s="44"/>
+      <c r="F59" s="45"/>
+      <c r="G59" s="45"/>
+      <c r="H59" s="45"/>
+      <c r="I59" s="45"/>
+      <c r="J59" s="45"/>
       <c r="K59" s="46"/>
       <c r="L59" s="46"/>
       <c r="P59" s="30"/>
-      <c r="S59" s="42"/>
-      <c r="T59" s="42"/>
-      <c r="U59" s="42"/>
-      <c r="V59" s="42"/>
+      <c r="S59" s="44"/>
+      <c r="T59" s="44"/>
+      <c r="U59" s="44"/>
+      <c r="V59" s="44"/>
       <c r="Y59" s="30"/>
       <c r="Z59" s="30"/>
       <c r="AA59" s="30"/>
       <c r="AB59" s="30"/>
       <c r="AC59" s="30"/>
-      <c r="AH59" s="42"/>
-      <c r="AI59" s="42"/>
-      <c r="AJ59" s="42"/>
-      <c r="AK59" s="42"/>
-      <c r="AL59" s="42"/>
-      <c r="AM59" s="42"/>
+      <c r="AH59" s="44"/>
+      <c r="AI59" s="44"/>
+      <c r="AJ59" s="44"/>
+      <c r="AK59" s="44"/>
+      <c r="AL59" s="44"/>
+      <c r="AM59" s="44"/>
       <c r="AN59" s="30"/>
       <c r="AO59" s="30"/>
       <c r="AP59" s="30"/>
@@ -12224,14 +13756,14 @@
       <c r="AR59" s="29"/>
       <c r="AS59" s="29"/>
       <c r="AT59" s="29"/>
-      <c r="BA59" s="44" t="s">
+      <c r="BA59" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="BB59" s="44"/>
-      <c r="BC59" s="44"/>
-      <c r="BD59" s="44"/>
-      <c r="BE59" s="44"/>
-      <c r="BF59" s="44"/>
+      <c r="BB59" s="45"/>
+      <c r="BC59" s="45"/>
+      <c r="BD59" s="45"/>
+      <c r="BE59" s="45"/>
+      <c r="BF59" s="45"/>
       <c r="BG59" s="46"/>
       <c r="BH59" s="46"/>
       <c r="CL59" s="29"/>
@@ -12245,19 +13777,19 @@
       <c r="CT59" s="29"/>
     </row>
     <row r="60" spans="4:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E60" s="44"/>
-      <c r="F60" s="44"/>
-      <c r="G60" s="44"/>
-      <c r="H60" s="44"/>
-      <c r="I60" s="44"/>
-      <c r="J60" s="44"/>
+      <c r="E60" s="45"/>
+      <c r="F60" s="45"/>
+      <c r="G60" s="45"/>
+      <c r="H60" s="45"/>
+      <c r="I60" s="45"/>
+      <c r="J60" s="45"/>
       <c r="K60" s="46"/>
       <c r="L60" s="46"/>
       <c r="P60" s="30"/>
-      <c r="S60" s="42"/>
-      <c r="T60" s="42"/>
-      <c r="U60" s="42"/>
-      <c r="V60" s="42"/>
+      <c r="S60" s="44"/>
+      <c r="T60" s="44"/>
+      <c r="U60" s="44"/>
+      <c r="V60" s="44"/>
       <c r="Y60" s="30"/>
       <c r="Z60" s="30"/>
       <c r="AA60" s="30"/>
@@ -12274,12 +13806,12 @@
       <c r="AR60" s="29"/>
       <c r="AS60" s="29"/>
       <c r="AT60" s="29"/>
-      <c r="BA60" s="44"/>
-      <c r="BB60" s="44"/>
-      <c r="BC60" s="44"/>
-      <c r="BD60" s="44"/>
-      <c r="BE60" s="44"/>
-      <c r="BF60" s="44"/>
+      <c r="BA60" s="45"/>
+      <c r="BB60" s="45"/>
+      <c r="BC60" s="45"/>
+      <c r="BD60" s="45"/>
+      <c r="BE60" s="45"/>
+      <c r="BF60" s="45"/>
       <c r="BG60" s="46"/>
       <c r="BH60" s="46"/>
       <c r="CL60" s="29"/>
@@ -12293,10 +13825,10 @@
       <c r="CT60" s="29"/>
     </row>
     <row r="61" spans="4:98" x14ac:dyDescent="0.15">
-      <c r="S61" s="42"/>
-      <c r="T61" s="42"/>
-      <c r="U61" s="42"/>
-      <c r="V61" s="42"/>
+      <c r="S61" s="44"/>
+      <c r="T61" s="44"/>
+      <c r="U61" s="44"/>
+      <c r="V61" s="44"/>
       <c r="AJ61" s="29"/>
       <c r="AK61" s="29"/>
       <c r="AL61" s="29"/>
@@ -12341,14 +13873,14 @@
       <c r="CT62" s="29"/>
     </row>
     <row r="63" spans="4:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="AH63" s="43" t="s">
+      <c r="AH63" s="48" t="s">
         <v>185</v>
       </c>
-      <c r="AI63" s="42"/>
-      <c r="AJ63" s="42"/>
-      <c r="AK63" s="42"/>
-      <c r="AL63" s="42"/>
-      <c r="AM63" s="42"/>
+      <c r="AI63" s="44"/>
+      <c r="AJ63" s="44"/>
+      <c r="AK63" s="44"/>
+      <c r="AL63" s="44"/>
+      <c r="AM63" s="44"/>
       <c r="AN63" s="29"/>
       <c r="AO63" s="29"/>
       <c r="AP63" s="29"/>
@@ -12375,20 +13907,20 @@
       <c r="CT63" s="29"/>
     </row>
     <row r="64" spans="4:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="R64" s="43" t="s">
+      <c r="R64" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="S64" s="42"/>
-      <c r="T64" s="42"/>
-      <c r="U64" s="42"/>
-      <c r="V64" s="42"/>
-      <c r="W64" s="42"/>
-      <c r="AH64" s="42"/>
-      <c r="AI64" s="42"/>
-      <c r="AJ64" s="42"/>
-      <c r="AK64" s="42"/>
-      <c r="AL64" s="42"/>
-      <c r="AM64" s="42"/>
+      <c r="S64" s="44"/>
+      <c r="T64" s="44"/>
+      <c r="U64" s="44"/>
+      <c r="V64" s="44"/>
+      <c r="W64" s="44"/>
+      <c r="AH64" s="44"/>
+      <c r="AI64" s="44"/>
+      <c r="AJ64" s="44"/>
+      <c r="AK64" s="44"/>
+      <c r="AL64" s="44"/>
+      <c r="AM64" s="44"/>
       <c r="AN64" s="29"/>
       <c r="AO64" s="29"/>
       <c r="AP64" s="29"/>
@@ -12414,27 +13946,27 @@
       <c r="CS64" s="29"/>
       <c r="CT64" s="29"/>
     </row>
-    <row r="65" spans="4:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D65" s="44" t="s">
+    <row r="65" spans="1:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D65" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="E65" s="45"/>
+      <c r="E65" s="50"/>
       <c r="F65" s="46"/>
       <c r="G65" s="46"/>
       <c r="H65" s="46"/>
       <c r="I65" s="46"/>
-      <c r="R65" s="42"/>
-      <c r="S65" s="42"/>
-      <c r="T65" s="42"/>
-      <c r="U65" s="42"/>
-      <c r="V65" s="42"/>
-      <c r="W65" s="42"/>
-      <c r="AH65" s="42"/>
-      <c r="AI65" s="42"/>
-      <c r="AJ65" s="42"/>
-      <c r="AK65" s="42"/>
-      <c r="AL65" s="42"/>
-      <c r="AM65" s="42"/>
+      <c r="R65" s="44"/>
+      <c r="S65" s="44"/>
+      <c r="T65" s="44"/>
+      <c r="U65" s="44"/>
+      <c r="V65" s="44"/>
+      <c r="W65" s="44"/>
+      <c r="AH65" s="44"/>
+      <c r="AI65" s="44"/>
+      <c r="AJ65" s="44"/>
+      <c r="AK65" s="44"/>
+      <c r="AL65" s="44"/>
+      <c r="AM65" s="44"/>
       <c r="AN65" s="29"/>
       <c r="AO65" s="29"/>
       <c r="AP65" s="29"/>
@@ -12442,10 +13974,10 @@
       <c r="AR65" s="29"/>
       <c r="AS65" s="29"/>
       <c r="AT65" s="29"/>
-      <c r="AZ65" s="44" t="s">
+      <c r="AZ65" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="BA65" s="45"/>
+      <c r="BA65" s="50"/>
       <c r="BB65" s="46"/>
       <c r="BC65" s="46"/>
       <c r="BD65" s="46"/>
@@ -12460,25 +13992,25 @@
       <c r="CS65" s="29"/>
       <c r="CT65" s="29"/>
     </row>
-    <row r="66" spans="4:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D66" s="45"/>
-      <c r="E66" s="45"/>
+    <row r="66" spans="1:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D66" s="50"/>
+      <c r="E66" s="50"/>
       <c r="F66" s="46"/>
       <c r="G66" s="46"/>
       <c r="H66" s="46"/>
       <c r="I66" s="46"/>
-      <c r="R66" s="42"/>
-      <c r="S66" s="42"/>
-      <c r="T66" s="42"/>
-      <c r="U66" s="42"/>
-      <c r="V66" s="42"/>
-      <c r="W66" s="42"/>
-      <c r="AH66" s="42"/>
-      <c r="AI66" s="42"/>
-      <c r="AJ66" s="42"/>
-      <c r="AK66" s="42"/>
-      <c r="AL66" s="42"/>
-      <c r="AM66" s="42"/>
+      <c r="R66" s="44"/>
+      <c r="S66" s="44"/>
+      <c r="T66" s="44"/>
+      <c r="U66" s="44"/>
+      <c r="V66" s="44"/>
+      <c r="W66" s="44"/>
+      <c r="AH66" s="44"/>
+      <c r="AI66" s="44"/>
+      <c r="AJ66" s="44"/>
+      <c r="AK66" s="44"/>
+      <c r="AL66" s="44"/>
+      <c r="AM66" s="44"/>
       <c r="AN66" s="29"/>
       <c r="AO66" s="29"/>
       <c r="AP66" s="29"/>
@@ -12486,8 +14018,8 @@
       <c r="AR66" s="29"/>
       <c r="AS66" s="29"/>
       <c r="AT66" s="29"/>
-      <c r="AZ66" s="45"/>
-      <c r="BA66" s="45"/>
+      <c r="AZ66" s="50"/>
+      <c r="BA66" s="50"/>
       <c r="BB66" s="46"/>
       <c r="BC66" s="46"/>
       <c r="BD66" s="46"/>
@@ -12502,13 +14034,13 @@
       <c r="CS66" s="29"/>
       <c r="CT66" s="29"/>
     </row>
-    <row r="67" spans="4:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="R67" s="42"/>
-      <c r="S67" s="42"/>
-      <c r="T67" s="42"/>
-      <c r="U67" s="42"/>
-      <c r="V67" s="42"/>
-      <c r="W67" s="42"/>
+    <row r="67" spans="1:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="R67" s="44"/>
+      <c r="S67" s="44"/>
+      <c r="T67" s="44"/>
+      <c r="U67" s="44"/>
+      <c r="V67" s="44"/>
+      <c r="W67" s="44"/>
       <c r="AJ67" s="29"/>
       <c r="AK67" s="29"/>
       <c r="AL67" s="29"/>
@@ -12530,7 +14062,7 @@
       <c r="CS67" s="29"/>
       <c r="CT67" s="29"/>
     </row>
-    <row r="68" spans="4:98" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:98" x14ac:dyDescent="0.15">
       <c r="AJ68" s="29"/>
       <c r="AK68" s="29"/>
       <c r="AL68" s="29"/>
@@ -12540,8 +14072,11 @@
       <c r="AP68" s="29"/>
       <c r="AQ68" s="29"/>
       <c r="AR68" s="29"/>
-      <c r="AS68" s="29"/>
-      <c r="AT68" s="29"/>
+      <c r="AS68" s="46" t="s">
+        <v>207</v>
+      </c>
+      <c r="AT68" s="46"/>
+      <c r="AU68" s="46"/>
       <c r="CL68" s="29"/>
       <c r="CM68" s="29"/>
       <c r="CN68" s="29"/>
@@ -12552,7 +14087,7 @@
       <c r="CS68" s="29"/>
       <c r="CT68" s="29"/>
     </row>
-    <row r="69" spans="4:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="AJ69" s="29"/>
       <c r="AK69" s="29"/>
       <c r="AL69" s="29"/>
@@ -12562,8 +14097,9 @@
       <c r="AP69" s="29"/>
       <c r="AQ69" s="29"/>
       <c r="AR69" s="29"/>
-      <c r="AS69" s="29"/>
-      <c r="AT69" s="29"/>
+      <c r="AS69" s="46"/>
+      <c r="AT69" s="46"/>
+      <c r="AU69" s="46"/>
       <c r="BU69" s="30"/>
       <c r="BV69" s="31"/>
       <c r="BW69" s="29"/>
@@ -12580,7 +14116,7 @@
       <c r="CS69" s="29"/>
       <c r="CT69" s="29"/>
     </row>
-    <row r="70" spans="4:98" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:98" x14ac:dyDescent="0.15">
       <c r="AJ70" s="29"/>
       <c r="AK70" s="29"/>
       <c r="AL70" s="29"/>
@@ -12608,8 +14144,8 @@
       <c r="CS70" s="29"/>
       <c r="CT70" s="29"/>
     </row>
-    <row r="71" spans="4:98" x14ac:dyDescent="0.15">
-      <c r="R71" s="44" t="s">
+    <row r="71" spans="1:98" x14ac:dyDescent="0.15">
+      <c r="R71" s="45" t="s">
         <v>184</v>
       </c>
       <c r="S71" s="46"/>
@@ -12617,18 +14153,20 @@
       <c r="U71" s="46"/>
       <c r="V71" s="46"/>
       <c r="W71" s="46"/>
-      <c r="AH71" s="51" t="s">
+      <c r="AH71" s="57" t="s">
         <v>186</v>
       </c>
-      <c r="AI71" s="42"/>
-      <c r="AJ71" s="42"/>
-      <c r="AK71" s="42"/>
-      <c r="AL71" s="42"/>
-      <c r="AM71" s="42"/>
+      <c r="AI71" s="44"/>
+      <c r="AJ71" s="44"/>
+      <c r="AK71" s="44"/>
+      <c r="AL71" s="44"/>
+      <c r="AM71" s="44"/>
       <c r="AN71" s="29"/>
       <c r="AO71" s="29"/>
       <c r="AP71" s="29"/>
-      <c r="AQ71" s="29"/>
+      <c r="AQ71" s="47" t="s">
+        <v>204</v>
+      </c>
       <c r="AR71" s="29"/>
       <c r="AS71" s="29"/>
       <c r="AT71" s="29"/>
@@ -12642,11 +14180,11 @@
       <c r="CS71" s="29"/>
       <c r="CT71" s="29"/>
     </row>
-    <row r="72" spans="4:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D72" s="44" t="s">
+    <row r="72" spans="1:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D72" s="45" t="s">
         <v>160</v>
       </c>
-      <c r="E72" s="45"/>
+      <c r="E72" s="50"/>
       <c r="F72" s="46"/>
       <c r="G72" s="46"/>
       <c r="H72" s="46"/>
@@ -12657,23 +14195,23 @@
       <c r="U72" s="46"/>
       <c r="V72" s="46"/>
       <c r="W72" s="46"/>
-      <c r="AH72" s="42"/>
-      <c r="AI72" s="42"/>
-      <c r="AJ72" s="42"/>
-      <c r="AK72" s="42"/>
-      <c r="AL72" s="42"/>
-      <c r="AM72" s="42"/>
+      <c r="AH72" s="44"/>
+      <c r="AI72" s="44"/>
+      <c r="AJ72" s="44"/>
+      <c r="AK72" s="44"/>
+      <c r="AL72" s="44"/>
+      <c r="AM72" s="44"/>
       <c r="AN72" s="29"/>
       <c r="AO72" s="29"/>
       <c r="AP72" s="29"/>
-      <c r="AQ72" s="29"/>
+      <c r="AQ72" s="46"/>
       <c r="AR72" s="29"/>
       <c r="AS72" s="29"/>
       <c r="AT72" s="29"/>
-      <c r="AZ72" s="44" t="s">
+      <c r="AZ72" s="45" t="s">
         <v>160</v>
       </c>
-      <c r="BA72" s="45"/>
+      <c r="BA72" s="50"/>
       <c r="BB72" s="46"/>
       <c r="BC72" s="46"/>
       <c r="BD72" s="46"/>
@@ -12688,9 +14226,9 @@
       <c r="CS72" s="29"/>
       <c r="CT72" s="29"/>
     </row>
-    <row r="73" spans="4:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D73" s="45"/>
-      <c r="E73" s="45"/>
+    <row r="73" spans="1:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D73" s="50"/>
+      <c r="E73" s="50"/>
       <c r="F73" s="46"/>
       <c r="G73" s="46"/>
       <c r="H73" s="46"/>
@@ -12701,12 +14239,12 @@
       <c r="U73" s="46"/>
       <c r="V73" s="46"/>
       <c r="W73" s="46"/>
-      <c r="AH73" s="42"/>
-      <c r="AI73" s="42"/>
-      <c r="AJ73" s="42"/>
-      <c r="AK73" s="42"/>
-      <c r="AL73" s="42"/>
-      <c r="AM73" s="42"/>
+      <c r="AH73" s="44"/>
+      <c r="AI73" s="44"/>
+      <c r="AJ73" s="44"/>
+      <c r="AK73" s="44"/>
+      <c r="AL73" s="44"/>
+      <c r="AM73" s="44"/>
       <c r="AN73" s="29"/>
       <c r="AO73" s="29"/>
       <c r="AP73" s="29"/>
@@ -12714,18 +14252,18 @@
       <c r="AR73" s="29"/>
       <c r="AS73" s="29"/>
       <c r="AT73" s="29"/>
-      <c r="AZ73" s="45"/>
-      <c r="BA73" s="45"/>
+      <c r="AZ73" s="50"/>
+      <c r="BA73" s="50"/>
       <c r="BB73" s="46"/>
       <c r="BC73" s="46"/>
       <c r="BD73" s="46"/>
       <c r="BE73" s="46"/>
-      <c r="BW73" s="54" t="s">
+      <c r="BW73" s="52" t="s">
         <v>194</v>
       </c>
-      <c r="BX73" s="42"/>
-      <c r="BY73" s="42"/>
-      <c r="BZ73" s="42"/>
+      <c r="BX73" s="44"/>
+      <c r="BY73" s="44"/>
+      <c r="BZ73" s="44"/>
       <c r="CL73" s="31"/>
       <c r="CM73" s="31"/>
       <c r="CN73" s="29"/>
@@ -12736,19 +14274,19 @@
       <c r="CS73" s="29"/>
       <c r="CT73" s="29"/>
     </row>
-    <row r="74" spans="4:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="R74" s="46"/>
       <c r="S74" s="46"/>
       <c r="T74" s="46"/>
       <c r="U74" s="46"/>
       <c r="V74" s="46"/>
       <c r="W74" s="46"/>
-      <c r="AH74" s="42"/>
-      <c r="AI74" s="42"/>
-      <c r="AJ74" s="42"/>
-      <c r="AK74" s="42"/>
-      <c r="AL74" s="42"/>
-      <c r="AM74" s="42"/>
+      <c r="AH74" s="44"/>
+      <c r="AI74" s="44"/>
+      <c r="AJ74" s="44"/>
+      <c r="AK74" s="44"/>
+      <c r="AL74" s="44"/>
+      <c r="AM74" s="44"/>
       <c r="AN74" s="29"/>
       <c r="AO74" s="29"/>
       <c r="AP74" s="29"/>
@@ -12756,10 +14294,10 @@
       <c r="AR74" s="29"/>
       <c r="AS74" s="29"/>
       <c r="AT74" s="29"/>
-      <c r="BW74" s="42"/>
-      <c r="BX74" s="42"/>
-      <c r="BY74" s="42"/>
-      <c r="BZ74" s="42"/>
+      <c r="BW74" s="44"/>
+      <c r="BX74" s="44"/>
+      <c r="BY74" s="44"/>
+      <c r="BZ74" s="44"/>
       <c r="CL74" s="29"/>
       <c r="CM74" s="29"/>
       <c r="CN74" s="29"/>
@@ -12770,7 +14308,7 @@
       <c r="CS74" s="29"/>
       <c r="CT74" s="29"/>
     </row>
-    <row r="75" spans="4:98" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:98" x14ac:dyDescent="0.15">
       <c r="AJ75" s="29"/>
       <c r="AK75" s="29"/>
       <c r="AL75" s="29"/>
@@ -12792,7 +14330,12 @@
       <c r="CS75" s="29"/>
       <c r="CT75" s="29"/>
     </row>
-    <row r="76" spans="4:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AC76" s="46" t="s">
+        <v>207</v>
+      </c>
+      <c r="AD76" s="46"/>
+      <c r="AE76" s="46"/>
       <c r="AJ76" s="29"/>
       <c r="AK76" s="29"/>
       <c r="AL76" s="29"/>
@@ -12804,7 +14347,7 @@
       <c r="AR76" s="29"/>
       <c r="AS76" s="29"/>
       <c r="AT76" s="29"/>
-      <c r="BU76" s="43" t="s">
+      <c r="BU76" s="48" t="s">
         <v>201</v>
       </c>
       <c r="BV76" s="46"/>
@@ -12823,7 +14366,10 @@
       <c r="CS76" s="29"/>
       <c r="CT76" s="29"/>
     </row>
-    <row r="77" spans="4:98" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:98" x14ac:dyDescent="0.15">
+      <c r="AC77" s="46"/>
+      <c r="AD77" s="46"/>
+      <c r="AE77" s="46"/>
       <c r="AJ77" s="29"/>
       <c r="AK77" s="29"/>
       <c r="AL77" s="29"/>
@@ -12852,22 +14398,25 @@
       <c r="CS77" s="29"/>
       <c r="CT77" s="29"/>
     </row>
-    <row r="78" spans="4:98" x14ac:dyDescent="0.15">
-      <c r="AH78" s="51" t="s">
+    <row r="78" spans="1:98" x14ac:dyDescent="0.15">
+      <c r="AH78" s="57" t="s">
         <v>187</v>
       </c>
-      <c r="AI78" s="42"/>
-      <c r="AJ78" s="42"/>
-      <c r="AK78" s="42"/>
-      <c r="AL78" s="42"/>
-      <c r="AM78" s="42"/>
+      <c r="AI78" s="44"/>
+      <c r="AJ78" s="44"/>
+      <c r="AK78" s="44"/>
+      <c r="AL78" s="44"/>
+      <c r="AM78" s="44"/>
       <c r="AN78" s="29"/>
       <c r="AO78" s="29"/>
       <c r="AP78" s="29"/>
       <c r="AQ78" s="29"/>
       <c r="AR78" s="29"/>
-      <c r="AS78" s="29"/>
-      <c r="AT78" s="29"/>
+      <c r="AS78" s="46" t="s">
+        <v>206</v>
+      </c>
+      <c r="AT78" s="46"/>
+      <c r="AU78" s="46"/>
       <c r="BU78" s="46"/>
       <c r="BV78" s="46"/>
       <c r="BW78" s="46"/>
@@ -12885,28 +14434,38 @@
       <c r="CS78" s="29"/>
       <c r="CT78" s="29"/>
     </row>
-    <row r="79" spans="4:98" x14ac:dyDescent="0.15">
-      <c r="R79" s="43" t="s">
+    <row r="79" spans="1:98" x14ac:dyDescent="0.15">
+      <c r="N79" s="47" t="s">
+        <v>205</v>
+      </c>
+      <c r="R79" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="S79" s="42"/>
-      <c r="T79" s="42"/>
-      <c r="U79" s="42"/>
-      <c r="V79" s="42"/>
-      <c r="W79" s="42"/>
-      <c r="AH79" s="42"/>
-      <c r="AI79" s="42"/>
-      <c r="AJ79" s="42"/>
-      <c r="AK79" s="42"/>
-      <c r="AL79" s="42"/>
-      <c r="AM79" s="42"/>
+      <c r="S79" s="44"/>
+      <c r="T79" s="44"/>
+      <c r="U79" s="44"/>
+      <c r="V79" s="44"/>
+      <c r="W79" s="44"/>
+      <c r="AA79" s="47" t="s">
+        <v>205</v>
+      </c>
+      <c r="AH79" s="44"/>
+      <c r="AI79" s="44"/>
+      <c r="AJ79" s="44"/>
+      <c r="AK79" s="44"/>
+      <c r="AL79" s="44"/>
+      <c r="AM79" s="44"/>
       <c r="AN79" s="29"/>
       <c r="AO79" s="29"/>
       <c r="AP79" s="29"/>
       <c r="AQ79" s="29"/>
       <c r="AR79" s="29"/>
-      <c r="AS79" s="29"/>
-      <c r="AT79" s="29"/>
+      <c r="AS79" s="46"/>
+      <c r="AT79" s="46"/>
+      <c r="AU79" s="46"/>
+      <c r="BD79" s="47" t="s">
+        <v>204</v>
+      </c>
       <c r="BU79" s="46"/>
       <c r="BV79" s="46"/>
       <c r="BW79" s="46"/>
@@ -12924,27 +14483,29 @@
       <c r="CS79" s="29"/>
       <c r="CT79" s="29"/>
     </row>
-    <row r="80" spans="4:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D80" s="44" t="s">
+    <row r="80" spans="1:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A80" s="45" t="s">
         <v>161</v>
       </c>
-      <c r="E80" s="45"/>
-      <c r="F80" s="46"/>
-      <c r="G80" s="46"/>
-      <c r="H80" s="46"/>
-      <c r="I80" s="46"/>
-      <c r="R80" s="42"/>
-      <c r="S80" s="42"/>
-      <c r="T80" s="42"/>
-      <c r="U80" s="42"/>
-      <c r="V80" s="42"/>
-      <c r="W80" s="42"/>
-      <c r="AH80" s="42"/>
-      <c r="AI80" s="42"/>
-      <c r="AJ80" s="42"/>
-      <c r="AK80" s="42"/>
-      <c r="AL80" s="42"/>
-      <c r="AM80" s="42"/>
+      <c r="B80" s="46"/>
+      <c r="C80" s="46"/>
+      <c r="D80" s="46"/>
+      <c r="E80" s="32"/>
+      <c r="F80" s="32"/>
+      <c r="N80" s="46"/>
+      <c r="R80" s="44"/>
+      <c r="S80" s="44"/>
+      <c r="T80" s="44"/>
+      <c r="U80" s="44"/>
+      <c r="V80" s="44"/>
+      <c r="W80" s="44"/>
+      <c r="AA80" s="46"/>
+      <c r="AH80" s="44"/>
+      <c r="AI80" s="44"/>
+      <c r="AJ80" s="44"/>
+      <c r="AK80" s="44"/>
+      <c r="AL80" s="44"/>
+      <c r="AM80" s="44"/>
       <c r="AN80" s="29"/>
       <c r="AO80" s="29"/>
       <c r="AP80" s="29"/>
@@ -12952,14 +14513,14 @@
       <c r="AR80" s="29"/>
       <c r="AS80" s="29"/>
       <c r="AT80" s="29"/>
-      <c r="AZ80" s="44" t="s">
+      <c r="AZ80" s="45" t="s">
         <v>161</v>
       </c>
-      <c r="BA80" s="45"/>
+      <c r="BA80" s="46"/>
       <c r="BB80" s="46"/>
       <c r="BC80" s="46"/>
       <c r="BD80" s="46"/>
-      <c r="BE80" s="46"/>
+      <c r="BE80" s="33"/>
       <c r="CL80" s="30"/>
       <c r="CM80" s="31"/>
       <c r="CN80" s="29"/>
@@ -12970,25 +14531,25 @@
       <c r="CS80" s="29"/>
       <c r="CT80" s="29"/>
     </row>
-    <row r="81" spans="4:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D81" s="45"/>
-      <c r="E81" s="45"/>
-      <c r="F81" s="46"/>
-      <c r="G81" s="46"/>
-      <c r="H81" s="46"/>
-      <c r="I81" s="46"/>
-      <c r="R81" s="42"/>
-      <c r="S81" s="42"/>
-      <c r="T81" s="42"/>
-      <c r="U81" s="42"/>
-      <c r="V81" s="42"/>
-      <c r="W81" s="42"/>
-      <c r="AH81" s="42"/>
-      <c r="AI81" s="42"/>
-      <c r="AJ81" s="42"/>
-      <c r="AK81" s="42"/>
-      <c r="AL81" s="42"/>
-      <c r="AM81" s="42"/>
+    <row r="81" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A81" s="46"/>
+      <c r="B81" s="46"/>
+      <c r="C81" s="46"/>
+      <c r="D81" s="46"/>
+      <c r="E81" s="32"/>
+      <c r="F81" s="32"/>
+      <c r="R81" s="44"/>
+      <c r="S81" s="44"/>
+      <c r="T81" s="44"/>
+      <c r="U81" s="44"/>
+      <c r="V81" s="44"/>
+      <c r="W81" s="44"/>
+      <c r="AH81" s="44"/>
+      <c r="AI81" s="44"/>
+      <c r="AJ81" s="44"/>
+      <c r="AK81" s="44"/>
+      <c r="AL81" s="44"/>
+      <c r="AM81" s="44"/>
       <c r="AN81" s="29"/>
       <c r="AO81" s="29"/>
       <c r="AP81" s="29"/>
@@ -12996,12 +14557,12 @@
       <c r="AR81" s="29"/>
       <c r="AS81" s="29"/>
       <c r="AT81" s="29"/>
-      <c r="AZ81" s="45"/>
-      <c r="BA81" s="45"/>
+      <c r="AZ81" s="46"/>
+      <c r="BA81" s="46"/>
       <c r="BB81" s="46"/>
       <c r="BC81" s="46"/>
-      <c r="BD81" s="46"/>
-      <c r="BE81" s="46"/>
+      <c r="BD81" s="33"/>
+      <c r="BE81" s="33"/>
       <c r="CL81" s="31"/>
       <c r="CM81" s="31"/>
       <c r="CN81" s="29"/>
@@ -13012,13 +14573,13 @@
       <c r="CS81" s="29"/>
       <c r="CT81" s="29"/>
     </row>
-    <row r="82" spans="4:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="R82" s="42"/>
-      <c r="S82" s="42"/>
-      <c r="T82" s="42"/>
-      <c r="U82" s="42"/>
-      <c r="V82" s="42"/>
-      <c r="W82" s="42"/>
+    <row r="82" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="R82" s="44"/>
+      <c r="S82" s="44"/>
+      <c r="T82" s="44"/>
+      <c r="U82" s="44"/>
+      <c r="V82" s="44"/>
+      <c r="W82" s="44"/>
       <c r="AJ82" s="29"/>
       <c r="AK82" s="29"/>
       <c r="AL82" s="29"/>
@@ -13040,7 +14601,7 @@
       <c r="CS82" s="29"/>
       <c r="CT82" s="29"/>
     </row>
-    <row r="83" spans="4:99" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:99" x14ac:dyDescent="0.15">
       <c r="AJ83" s="29"/>
       <c r="AK83" s="29"/>
       <c r="AL83" s="29"/>
@@ -13062,7 +14623,7 @@
       <c r="CS83" s="29"/>
       <c r="CT83" s="29"/>
     </row>
-    <row r="84" spans="4:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="AJ84" s="29"/>
       <c r="AK84" s="29"/>
       <c r="AL84" s="29"/>
@@ -13081,7 +14642,7 @@
       <c r="BY84" s="29"/>
       <c r="BZ84" s="29"/>
     </row>
-    <row r="85" spans="4:99" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:99" x14ac:dyDescent="0.15">
       <c r="BU85" s="31"/>
       <c r="BV85" s="31"/>
       <c r="BW85" s="29"/>
@@ -13089,7 +14650,17 @@
       <c r="BY85" s="29"/>
       <c r="BZ85" s="29"/>
     </row>
-    <row r="87" spans="4:99" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:99" x14ac:dyDescent="0.15">
+      <c r="AC86" s="46" t="s">
+        <v>206</v>
+      </c>
+      <c r="AD86" s="46"/>
+      <c r="AE86" s="46"/>
+    </row>
+    <row r="87" spans="1:99" x14ac:dyDescent="0.15">
+      <c r="AC87" s="46"/>
+      <c r="AD87" s="46"/>
+      <c r="AE87" s="46"/>
       <c r="AY87" s="29"/>
       <c r="AZ87" s="29"/>
       <c r="BA87" s="29"/>
@@ -13109,7 +14680,7 @@
       <c r="CR87" s="29"/>
       <c r="CS87" s="29"/>
     </row>
-    <row r="88" spans="4:99" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:99" x14ac:dyDescent="0.15">
       <c r="AY88" s="29"/>
       <c r="AZ88" s="29"/>
       <c r="BA88" s="29"/>
@@ -13129,7 +14700,7 @@
       <c r="CR88" s="29"/>
       <c r="CS88" s="29"/>
     </row>
-    <row r="89" spans="4:99" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:99" x14ac:dyDescent="0.15">
       <c r="BC89" s="29"/>
       <c r="BD89" s="29"/>
       <c r="BE89" s="29"/>
@@ -13147,15 +14718,15 @@
       <c r="CT89" s="29"/>
       <c r="CU89" s="29"/>
     </row>
-    <row r="90" spans="4:99" x14ac:dyDescent="0.15">
-      <c r="AH90" s="51" t="s">
+    <row r="90" spans="1:99" x14ac:dyDescent="0.15">
+      <c r="AH90" s="57" t="s">
         <v>188</v>
       </c>
-      <c r="AI90" s="42"/>
-      <c r="AJ90" s="42"/>
-      <c r="AK90" s="42"/>
-      <c r="AL90" s="42"/>
-      <c r="AM90" s="42"/>
+      <c r="AI90" s="44"/>
+      <c r="AJ90" s="44"/>
+      <c r="AK90" s="44"/>
+      <c r="AL90" s="44"/>
+      <c r="AM90" s="44"/>
       <c r="BC90" s="29"/>
       <c r="BD90" s="29"/>
       <c r="BE90" s="29"/>
@@ -13166,13 +14737,13 @@
       <c r="BJ90" s="29"/>
       <c r="BK90" s="29"/>
     </row>
-    <row r="91" spans="4:99" x14ac:dyDescent="0.15">
-      <c r="AH91" s="42"/>
-      <c r="AI91" s="42"/>
-      <c r="AJ91" s="42"/>
-      <c r="AK91" s="42"/>
-      <c r="AL91" s="42"/>
-      <c r="AM91" s="42"/>
+    <row r="91" spans="1:99" x14ac:dyDescent="0.15">
+      <c r="AH91" s="44"/>
+      <c r="AI91" s="44"/>
+      <c r="AJ91" s="44"/>
+      <c r="AK91" s="44"/>
+      <c r="AL91" s="44"/>
+      <c r="AM91" s="44"/>
       <c r="BC91" s="29"/>
       <c r="BD91" s="29"/>
       <c r="BE91" s="29"/>
@@ -13190,13 +14761,13 @@
       <c r="CG91" s="29"/>
       <c r="CH91" s="29"/>
     </row>
-    <row r="92" spans="4:99" x14ac:dyDescent="0.15">
-      <c r="AH92" s="42"/>
-      <c r="AI92" s="42"/>
-      <c r="AJ92" s="42"/>
-      <c r="AK92" s="42"/>
-      <c r="AL92" s="42"/>
-      <c r="AM92" s="42"/>
+    <row r="92" spans="1:99" x14ac:dyDescent="0.15">
+      <c r="AH92" s="44"/>
+      <c r="AI92" s="44"/>
+      <c r="AJ92" s="44"/>
+      <c r="AK92" s="44"/>
+      <c r="AL92" s="44"/>
+      <c r="AM92" s="44"/>
       <c r="BC92" s="29"/>
       <c r="BD92" s="29"/>
       <c r="BE92" s="29"/>
@@ -13207,13 +14778,13 @@
       <c r="BJ92" s="29"/>
       <c r="BK92" s="29"/>
     </row>
-    <row r="93" spans="4:99" x14ac:dyDescent="0.15">
-      <c r="AH93" s="42"/>
-      <c r="AI93" s="42"/>
-      <c r="AJ93" s="42"/>
-      <c r="AK93" s="42"/>
-      <c r="AL93" s="42"/>
-      <c r="AM93" s="42"/>
+    <row r="93" spans="1:99" x14ac:dyDescent="0.15">
+      <c r="AH93" s="44"/>
+      <c r="AI93" s="44"/>
+      <c r="AJ93" s="44"/>
+      <c r="AK93" s="44"/>
+      <c r="AL93" s="44"/>
+      <c r="AM93" s="44"/>
       <c r="BC93" s="29"/>
       <c r="BD93" s="29"/>
       <c r="BE93" s="29"/>
@@ -13224,136 +14795,172 @@
       <c r="BJ93" s="29"/>
       <c r="BK93" s="29"/>
     </row>
-    <row r="95" spans="4:99" x14ac:dyDescent="0.15">
-      <c r="BV95" s="43" t="s">
+    <row r="95" spans="1:99" x14ac:dyDescent="0.15">
+      <c r="BV95" s="48" t="s">
         <v>199</v>
       </c>
-      <c r="BW95" s="42"/>
-      <c r="BX95" s="42"/>
-      <c r="BY95" s="42"/>
-      <c r="BZ95" s="42"/>
-      <c r="CA95" s="42"/>
-      <c r="CB95" s="42"/>
+      <c r="BW95" s="44"/>
+      <c r="BX95" s="44"/>
+      <c r="BY95" s="44"/>
+      <c r="BZ95" s="44"/>
+      <c r="CA95" s="44"/>
+      <c r="CB95" s="44"/>
     </row>
-    <row r="96" spans="4:99" x14ac:dyDescent="0.15">
-      <c r="BV96" s="42"/>
-      <c r="BW96" s="42"/>
-      <c r="BX96" s="42"/>
-      <c r="BY96" s="42"/>
-      <c r="BZ96" s="42"/>
-      <c r="CA96" s="42"/>
-      <c r="CB96" s="42"/>
+    <row r="96" spans="1:99" x14ac:dyDescent="0.15">
+      <c r="BV96" s="44"/>
+      <c r="BW96" s="44"/>
+      <c r="BX96" s="44"/>
+      <c r="BY96" s="44"/>
+      <c r="BZ96" s="44"/>
+      <c r="CA96" s="44"/>
+      <c r="CB96" s="44"/>
     </row>
-    <row r="97" spans="34:74" x14ac:dyDescent="0.15">
-      <c r="AH97" s="43" t="s">
+    <row r="97" spans="30:74" x14ac:dyDescent="0.15">
+      <c r="AH97" s="48" t="s">
         <v>189</v>
       </c>
-      <c r="AI97" s="42"/>
-      <c r="AJ97" s="42"/>
-      <c r="AK97" s="42"/>
-      <c r="AL97" s="42"/>
-      <c r="AM97" s="42"/>
+      <c r="AI97" s="44"/>
+      <c r="AJ97" s="44"/>
+      <c r="AK97" s="44"/>
+      <c r="AL97" s="44"/>
+      <c r="AM97" s="44"/>
     </row>
-    <row r="98" spans="34:74" x14ac:dyDescent="0.15">
-      <c r="AH98" s="42"/>
-      <c r="AI98" s="42"/>
-      <c r="AJ98" s="42"/>
-      <c r="AK98" s="42"/>
-      <c r="AL98" s="42"/>
-      <c r="AM98" s="42"/>
+    <row r="98" spans="30:74" x14ac:dyDescent="0.15">
+      <c r="AH98" s="44"/>
+      <c r="AI98" s="44"/>
+      <c r="AJ98" s="44"/>
+      <c r="AK98" s="44"/>
+      <c r="AL98" s="44"/>
+      <c r="AM98" s="44"/>
     </row>
-    <row r="99" spans="34:74" x14ac:dyDescent="0.15">
-      <c r="AH99" s="42"/>
-      <c r="AI99" s="42"/>
-      <c r="AJ99" s="42"/>
-      <c r="AK99" s="42"/>
-      <c r="AL99" s="42"/>
-      <c r="AM99" s="42"/>
+    <row r="99" spans="30:74" x14ac:dyDescent="0.15">
+      <c r="AH99" s="44"/>
+      <c r="AI99" s="44"/>
+      <c r="AJ99" s="44"/>
+      <c r="AK99" s="44"/>
+      <c r="AL99" s="44"/>
+      <c r="AM99" s="44"/>
     </row>
-    <row r="100" spans="34:74" x14ac:dyDescent="0.15">
-      <c r="AH100" s="42"/>
-      <c r="AI100" s="42"/>
-      <c r="AJ100" s="42"/>
-      <c r="AK100" s="42"/>
-      <c r="AL100" s="42"/>
-      <c r="AM100" s="42"/>
+    <row r="100" spans="30:74" x14ac:dyDescent="0.15">
+      <c r="AH100" s="44"/>
+      <c r="AI100" s="44"/>
+      <c r="AJ100" s="44"/>
+      <c r="AK100" s="44"/>
+      <c r="AL100" s="44"/>
+      <c r="AM100" s="44"/>
     </row>
-    <row r="104" spans="34:74" x14ac:dyDescent="0.15">
-      <c r="BS104" s="49" t="s">
+    <row r="104" spans="30:74" x14ac:dyDescent="0.15">
+      <c r="BS104" s="51" t="s">
         <v>200</v>
       </c>
-      <c r="BT104" s="42"/>
-      <c r="BU104" s="42"/>
-      <c r="BV104" s="42"/>
+      <c r="BT104" s="44"/>
+      <c r="BU104" s="44"/>
+      <c r="BV104" s="44"/>
     </row>
-    <row r="105" spans="34:74" x14ac:dyDescent="0.15">
-      <c r="AH105" s="53" t="s">
+    <row r="105" spans="30:74" x14ac:dyDescent="0.15">
+      <c r="AD105" s="47" t="s">
+        <v>204</v>
+      </c>
+      <c r="AH105" s="55" t="s">
         <v>190</v>
       </c>
-      <c r="AI105" s="42"/>
-      <c r="AJ105" s="42"/>
-      <c r="AK105" s="42"/>
-      <c r="AL105" s="42"/>
-      <c r="AM105" s="42"/>
-      <c r="BS105" s="42"/>
-      <c r="BT105" s="42"/>
-      <c r="BU105" s="42"/>
-      <c r="BV105" s="42"/>
+      <c r="AI105" s="44"/>
+      <c r="AJ105" s="44"/>
+      <c r="AK105" s="44"/>
+      <c r="AL105" s="44"/>
+      <c r="AM105" s="44"/>
+      <c r="BS105" s="44"/>
+      <c r="BT105" s="44"/>
+      <c r="BU105" s="44"/>
+      <c r="BV105" s="44"/>
     </row>
-    <row r="106" spans="34:74" x14ac:dyDescent="0.15">
-      <c r="AH106" s="42"/>
-      <c r="AI106" s="42"/>
-      <c r="AJ106" s="42"/>
-      <c r="AK106" s="42"/>
-      <c r="AL106" s="42"/>
-      <c r="AM106" s="42"/>
-      <c r="BS106" s="42"/>
-      <c r="BT106" s="42"/>
-      <c r="BU106" s="42"/>
-      <c r="BV106" s="42"/>
+    <row r="106" spans="30:74" x14ac:dyDescent="0.15">
+      <c r="AD106" s="46"/>
+      <c r="AH106" s="44"/>
+      <c r="AI106" s="44"/>
+      <c r="AJ106" s="44"/>
+      <c r="AK106" s="44"/>
+      <c r="AL106" s="44"/>
+      <c r="AM106" s="44"/>
+      <c r="BS106" s="44"/>
+      <c r="BT106" s="44"/>
+      <c r="BU106" s="44"/>
+      <c r="BV106" s="44"/>
     </row>
-    <row r="107" spans="34:74" x14ac:dyDescent="0.15">
-      <c r="AH107" s="42"/>
-      <c r="AI107" s="42"/>
-      <c r="AJ107" s="42"/>
-      <c r="AK107" s="42"/>
-      <c r="AL107" s="42"/>
-      <c r="AM107" s="42"/>
-      <c r="BS107" s="42"/>
-      <c r="BT107" s="42"/>
-      <c r="BU107" s="42"/>
-      <c r="BV107" s="42"/>
+    <row r="107" spans="30:74" x14ac:dyDescent="0.15">
+      <c r="AH107" s="44"/>
+      <c r="AI107" s="44"/>
+      <c r="AJ107" s="44"/>
+      <c r="AK107" s="44"/>
+      <c r="AL107" s="44"/>
+      <c r="AM107" s="44"/>
+      <c r="BS107" s="44"/>
+      <c r="BT107" s="44"/>
+      <c r="BU107" s="44"/>
+      <c r="BV107" s="44"/>
     </row>
-    <row r="108" spans="34:74" x14ac:dyDescent="0.15">
-      <c r="AH108" s="42"/>
-      <c r="AI108" s="42"/>
-      <c r="AJ108" s="42"/>
-      <c r="AK108" s="42"/>
-      <c r="AL108" s="42"/>
-      <c r="AM108" s="42"/>
+    <row r="108" spans="30:74" x14ac:dyDescent="0.15">
+      <c r="AH108" s="44"/>
+      <c r="AI108" s="44"/>
+      <c r="AJ108" s="44"/>
+      <c r="AK108" s="44"/>
+      <c r="AL108" s="44"/>
+      <c r="AM108" s="44"/>
     </row>
+    <row r="125" spans="66:79" x14ac:dyDescent="0.15">
+      <c r="BN125" s="47" t="s">
+        <v>204</v>
+      </c>
+      <c r="CA125" s="47" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="126" spans="66:79" x14ac:dyDescent="0.15">
+      <c r="BN126" s="46"/>
+      <c r="CA126" s="46"/>
+    </row>
+    <row r="212" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <mergeCells count="66">
+  <mergeCells count="77">
+    <mergeCell ref="CA125:CA126"/>
+    <mergeCell ref="AZ80:BC81"/>
+    <mergeCell ref="BD79:BD80"/>
+    <mergeCell ref="BN125:BN126"/>
+    <mergeCell ref="C16:D17"/>
+    <mergeCell ref="D23:I24"/>
+    <mergeCell ref="D31:I32"/>
+    <mergeCell ref="D38:I39"/>
+    <mergeCell ref="E19:F20"/>
+    <mergeCell ref="D65:I66"/>
+    <mergeCell ref="D72:I73"/>
+    <mergeCell ref="D53:I54"/>
+    <mergeCell ref="D46:I47"/>
+    <mergeCell ref="E59:L60"/>
+    <mergeCell ref="R79:W82"/>
+    <mergeCell ref="R71:W74"/>
+    <mergeCell ref="AD105:AD106"/>
+    <mergeCell ref="R52:W55"/>
+    <mergeCell ref="R45:W48"/>
+    <mergeCell ref="S58:V61"/>
+    <mergeCell ref="R64:W67"/>
+    <mergeCell ref="T16:U17"/>
+    <mergeCell ref="U31:Z32"/>
+    <mergeCell ref="U23:Z24"/>
+    <mergeCell ref="V19:AB20"/>
     <mergeCell ref="Z42:AB43"/>
-    <mergeCell ref="M42:O43"/>
-    <mergeCell ref="CK16:CL17"/>
-    <mergeCell ref="CM19:CS20"/>
-    <mergeCell ref="CL31:CQ32"/>
-    <mergeCell ref="CL38:CU39"/>
-    <mergeCell ref="BV38:BX39"/>
-    <mergeCell ref="BW46:BZ47"/>
-    <mergeCell ref="BU41:BZ44"/>
-    <mergeCell ref="BV53:BX54"/>
-    <mergeCell ref="BU50:CA51"/>
-    <mergeCell ref="BW73:BZ74"/>
-    <mergeCell ref="CL46:CQ47"/>
-    <mergeCell ref="BV95:CB96"/>
-    <mergeCell ref="BS104:BV107"/>
-    <mergeCell ref="BU35:BZ36"/>
-    <mergeCell ref="BU57:BZ58"/>
-    <mergeCell ref="BU76:CA79"/>
-    <mergeCell ref="BT16:BU17"/>
-    <mergeCell ref="BV19:CB20"/>
+    <mergeCell ref="AL19:AU20"/>
+    <mergeCell ref="AZ46:BE47"/>
+    <mergeCell ref="AZ53:BE54"/>
+    <mergeCell ref="BA59:BH60"/>
+    <mergeCell ref="AZ65:BE66"/>
+    <mergeCell ref="AZ72:BE73"/>
+    <mergeCell ref="BA19:BG20"/>
+    <mergeCell ref="AZ23:BE24"/>
+    <mergeCell ref="AZ31:BE32"/>
+    <mergeCell ref="AZ38:BI39"/>
+    <mergeCell ref="AQ71:AQ72"/>
+    <mergeCell ref="AS68:AU69"/>
+    <mergeCell ref="AS78:AU79"/>
     <mergeCell ref="AH105:AM108"/>
     <mergeCell ref="AI28:AL31"/>
     <mergeCell ref="AI38:AL40"/>
@@ -13366,40 +14973,32 @@
     <mergeCell ref="AH78:AM81"/>
     <mergeCell ref="AH90:AM93"/>
     <mergeCell ref="AH97:AM100"/>
-    <mergeCell ref="AZ80:BE81"/>
-    <mergeCell ref="AL19:AU20"/>
-    <mergeCell ref="AZ46:BE47"/>
-    <mergeCell ref="AZ53:BE54"/>
-    <mergeCell ref="BA59:BH60"/>
-    <mergeCell ref="AZ65:BE66"/>
-    <mergeCell ref="AZ72:BE73"/>
+    <mergeCell ref="CL46:CQ47"/>
+    <mergeCell ref="BV95:CB96"/>
+    <mergeCell ref="BS104:BV107"/>
+    <mergeCell ref="BU35:BZ36"/>
+    <mergeCell ref="BU57:BZ58"/>
+    <mergeCell ref="BU76:CA79"/>
+    <mergeCell ref="BW46:BZ47"/>
+    <mergeCell ref="BU41:BZ44"/>
+    <mergeCell ref="BV53:BX54"/>
+    <mergeCell ref="BU50:CA51"/>
+    <mergeCell ref="BW73:BZ74"/>
+    <mergeCell ref="M42:O43"/>
+    <mergeCell ref="CK16:CL17"/>
+    <mergeCell ref="CM19:CS20"/>
+    <mergeCell ref="CL31:CQ32"/>
+    <mergeCell ref="CL38:CU39"/>
+    <mergeCell ref="BV38:BX39"/>
+    <mergeCell ref="BT16:BU17"/>
+    <mergeCell ref="BV19:CB20"/>
     <mergeCell ref="AY16:AZ17"/>
-    <mergeCell ref="BA19:BG20"/>
-    <mergeCell ref="AZ23:BE24"/>
-    <mergeCell ref="AZ31:BE32"/>
-    <mergeCell ref="AZ38:BI39"/>
-    <mergeCell ref="R79:W82"/>
-    <mergeCell ref="R71:W74"/>
     <mergeCell ref="AJ16:AK17"/>
-    <mergeCell ref="R52:W55"/>
-    <mergeCell ref="R45:W48"/>
-    <mergeCell ref="S58:V61"/>
-    <mergeCell ref="R64:W67"/>
-    <mergeCell ref="T16:U17"/>
-    <mergeCell ref="U31:Z32"/>
-    <mergeCell ref="U23:Z24"/>
-    <mergeCell ref="V19:AB20"/>
-    <mergeCell ref="D65:I66"/>
-    <mergeCell ref="D72:I73"/>
-    <mergeCell ref="D80:I81"/>
-    <mergeCell ref="D53:I54"/>
-    <mergeCell ref="D46:I47"/>
-    <mergeCell ref="E59:L60"/>
-    <mergeCell ref="C16:D17"/>
-    <mergeCell ref="D23:I24"/>
-    <mergeCell ref="D31:I32"/>
-    <mergeCell ref="D38:I39"/>
-    <mergeCell ref="E19:F20"/>
+    <mergeCell ref="A80:D81"/>
+    <mergeCell ref="AC76:AE77"/>
+    <mergeCell ref="AA79:AA80"/>
+    <mergeCell ref="AC86:AE87"/>
+    <mergeCell ref="N79:N80"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>